<commit_message>
Updates (Angepasste Constraints bei Netzanschluss)
</commit_message>
<xml_diff>
--- a/output/results.xlsx
+++ b/output/results.xlsx
@@ -20,7 +20,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -43,15 +43,6 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <b val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -61,7 +52,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -69,47 +60,22 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -477,10 +443,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -489,244 +455,89 @@
     <col width="10.83203125" customWidth="1" min="3" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="112" customFormat="1" customHeight="1" s="1">
-      <c r="B1" s="8" t="inlineStr">
+    <row r="1" ht="115" customFormat="1" customHeight="1" s="6">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>Base</t>
         </is>
       </c>
-      <c r="C1" s="8" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
-          <t>Bidirektional</t>
+          <t>Netzanschluss-90</t>
         </is>
       </c>
-      <c r="D1" s="8" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
-          <t>Cluster-1</t>
+          <t>Netzanschluss-80</t>
         </is>
       </c>
-      <c r="E1" s="8" t="inlineStr">
+      <c r="E1" s="6" t="inlineStr">
         <is>
-          <t>Cluster-3</t>
+          <t>Netzanschluss-70</t>
         </is>
       </c>
-      <c r="F1" s="8" t="inlineStr">
+      <c r="F1" s="6" t="inlineStr">
         <is>
-          <t>Leistung-NCS-110</t>
+          <t>Netzanschluss-60</t>
         </is>
       </c>
-      <c r="G1" s="8" t="inlineStr">
+      <c r="G1" s="6" t="inlineStr">
         <is>
-          <t>Leistung-NCS-120</t>
+          <t>Netzanschluss-50</t>
         </is>
       </c>
-      <c r="H1" s="8" t="inlineStr">
+      <c r="H1" s="6" t="inlineStr">
         <is>
-          <t>Leistung-NCS-130</t>
+          <t>Netzanschluss-40</t>
         </is>
       </c>
-      <c r="I1" s="8" t="inlineStr">
+      <c r="I1" s="6" t="inlineStr">
         <is>
-          <t>Leistung-NCS-140</t>
+          <t>Netzanschluss-30</t>
         </is>
       </c>
-      <c r="J1" s="8" t="inlineStr">
+      <c r="J1" s="6" t="inlineStr">
         <is>
-          <t>Leistung-HPC-110</t>
+          <t>Netzanschluss-20</t>
         </is>
       </c>
-      <c r="K1" s="8" t="inlineStr">
+      <c r="K1" s="6" t="inlineStr">
         <is>
-          <t>Leistung-HPC-120</t>
+          <t>Netzanschluss-10</t>
         </is>
       </c>
-      <c r="L1" s="8" t="inlineStr">
-        <is>
-          <t>Leistung-HPC-130</t>
-        </is>
-      </c>
-      <c r="M1" s="8" t="inlineStr">
-        <is>
-          <t>Leistung-HPC-140</t>
-        </is>
-      </c>
-      <c r="N1" s="8" t="inlineStr">
-        <is>
-          <t>Leistung-MCS-110</t>
-        </is>
-      </c>
-      <c r="O1" s="8" t="inlineStr">
-        <is>
-          <t>Leistung-MCS-120</t>
-        </is>
-      </c>
-      <c r="P1" s="8" t="inlineStr">
-        <is>
-          <t>Leistung-MCS-130</t>
-        </is>
-      </c>
-      <c r="Q1" s="8" t="inlineStr">
-        <is>
-          <t>Leistung-MCS-140</t>
-        </is>
-      </c>
-      <c r="R1" s="8" t="inlineStr">
-        <is>
-          <t>Ladequoten-NCS-25</t>
-        </is>
-      </c>
-      <c r="S1" s="8" t="inlineStr">
-        <is>
-          <t>Ladequoten-NCS-75</t>
-        </is>
-      </c>
-      <c r="T1" s="8" t="inlineStr">
-        <is>
-          <t>Ladequoten-NCS-50</t>
-        </is>
-      </c>
-      <c r="U1" s="8" t="inlineStr">
-        <is>
-          <t>Ladequoten-HPC-25</t>
-        </is>
-      </c>
-      <c r="V1" s="8" t="inlineStr">
-        <is>
-          <t>Ladequoten-HPC-75</t>
-        </is>
-      </c>
-      <c r="W1" s="8" t="inlineStr">
-        <is>
-          <t>Ladequoten-HPC-50</t>
-        </is>
-      </c>
-      <c r="X1" s="8" t="inlineStr">
-        <is>
-          <t>Ladequoten-MCS-25</t>
-        </is>
-      </c>
-      <c r="Y1" s="8" t="inlineStr">
-        <is>
-          <t>Ladequoten-MCS-75</t>
-        </is>
-      </c>
-      <c r="Z1" s="8" t="inlineStr">
-        <is>
-          <t>Ladequoten-MCS-50</t>
-        </is>
-      </c>
-      <c r="AA1" s="8" t="inlineStr">
-        <is>
-          <t>Pausenzeiten-60</t>
-        </is>
-      </c>
-      <c r="AB1" s="8" t="inlineStr">
-        <is>
-          <t>Pausenzeiten-75</t>
-        </is>
-      </c>
-      <c r="AC1" s="8" t="inlineStr">
-        <is>
-          <t>Pausenzeiten-600</t>
-        </is>
-      </c>
-      <c r="AD1" s="8" t="inlineStr">
-        <is>
-          <t>Pausenzeiten-660</t>
-        </is>
-      </c>
     </row>
-    <row r="2" ht="13" customFormat="1" customHeight="1" s="1">
-      <c r="B2" s="1" t="n">
+    <row r="2" ht="23" customFormat="1" customHeight="1" s="1">
+      <c r="B2" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D2" t="n">
-        <v>3</v>
+      <c r="C2" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="D2" s="6" t="n">
+        <v>31</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="F2" t="n">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="G2" t="n">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="H2" t="n">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="I2" t="n">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="J2" t="n">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="K2" t="n">
-        <v>10</v>
-      </c>
-      <c r="L2" t="n">
-        <v>11</v>
-      </c>
-      <c r="M2" t="n">
-        <v>12</v>
-      </c>
-      <c r="N2" t="n">
-        <v>13</v>
-      </c>
-      <c r="O2" t="n">
-        <v>14</v>
-      </c>
-      <c r="P2" t="n">
-        <v>15</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>16</v>
-      </c>
-      <c r="R2" t="n">
-        <v>17</v>
-      </c>
-      <c r="S2" t="n">
-        <v>18</v>
-      </c>
-      <c r="T2" t="n">
-        <v>19</v>
-      </c>
-      <c r="U2" t="n">
-        <v>20</v>
-      </c>
-      <c r="V2" t="n">
-        <v>21</v>
-      </c>
-      <c r="W2" t="n">
-        <v>22</v>
-      </c>
-      <c r="X2" t="n">
-        <v>23</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>24</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>25</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>26</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>27</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>28</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" t="inlineStr"/>
+        <v>38</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
@@ -734,368 +545,137 @@
           <t>Energieflexibilität</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
     </row>
-    <row r="5" customFormat="1" s="5">
-      <c r="A5" s="5" t="inlineStr">
+    <row r="5" customFormat="1" s="3">
+      <c r="A5" s="3" t="inlineStr">
         <is>
           <t>EFI</t>
         </is>
       </c>
-      <c r="B5" s="5" t="n">
-        <v>0.4138499118937396</v>
+      <c r="B5" t="n">
+        <v>0.413849911893739</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4138499118937386</v>
+        <v>0.4138499118937384</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4296654702291796</v>
+        <v>0.4138499118937384</v>
       </c>
       <c r="E5" t="n">
-        <v>0.4091680118356128</v>
+        <v>0.4138499118937384</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4372324529219176</v>
+        <v>0.4138499118937384</v>
       </c>
       <c r="G5" t="n">
-        <v>0.4588210187015173</v>
+        <v>0.4138499118937384</v>
       </c>
       <c r="H5" t="n">
-        <v>0.4788144401430489</v>
+        <v>0.4138499118937384</v>
       </c>
       <c r="I5" t="n">
-        <v>0.4973832124072979</v>
+        <v>0.4138499118937384</v>
       </c>
       <c r="J5" t="n">
-        <v>0.4195770901881732</v>
+        <v>0.4138499118937383</v>
       </c>
       <c r="K5" t="n">
-        <v>0.4251934327635213</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.4307021262220838</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.4359532572236464</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.4410077403037785</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0.4657604223783897</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0.4884139161738593</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0.5092243962653318</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0.4705490644708274</v>
-      </c>
-      <c r="S5" t="n">
-        <v>0.4285603706027767</v>
-      </c>
-      <c r="T5" t="n">
-        <v>0.4483646805898121</v>
-      </c>
-      <c r="U5" t="n">
-        <v>0.427557765058554</v>
-      </c>
-      <c r="V5" t="n">
-        <v>0.4170899697577152</v>
-      </c>
-      <c r="W5" t="n">
-        <v>0.4200625800415475</v>
-      </c>
-      <c r="X5" t="n">
-        <v>0.3328316146580053</v>
-      </c>
-      <c r="Y5" t="n">
-        <v>0.4022614121945752</v>
-      </c>
-      <c r="Z5" t="n">
-        <v>0.3830167782049651</v>
-      </c>
-      <c r="AA5" t="n">
-        <v>0.413849911893739</v>
-      </c>
-      <c r="AB5" t="n">
-        <v>0.413849911893739</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>0.413849911893739</v>
-      </c>
-      <c r="AD5" t="n">
-        <v>0.413849911893739</v>
+        <v>0.5093155213214242</v>
       </c>
     </row>
-    <row r="6" customFormat="1" s="3">
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="n">
-        <v>-8.881784197001252e-16</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.03821568612415582</v>
-      </c>
-      <c r="E6" t="n">
-        <v>-0.01131303867313216</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.05650005075797226</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.1086652564500852</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.1569760591515852</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.2018444322757451</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.01383878099243074</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.02740974576477595</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.04072059421549867</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.0534090855034004</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.06562240954883336</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0.1254331799833255</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0.1801716084435594</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>0.2304566985049434</v>
-      </c>
-      <c r="R6" t="n">
-        <v>0.1370041431630089</v>
-      </c>
-      <c r="S6" t="n">
-        <v>0.03554539529010414</v>
-      </c>
-      <c r="T6" t="n">
-        <v>0.08339924137747601</v>
-      </c>
-      <c r="U6" t="n">
-        <v>0.03312276448746632</v>
-      </c>
-      <c r="V6" t="n">
-        <v>0.007829065008495339</v>
-      </c>
-      <c r="W6" t="n">
-        <v>0.01501188708577939</v>
-      </c>
-      <c r="X6" t="n">
-        <v>-0.1957673419936262</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>-0.02800169666857222</v>
-      </c>
-      <c r="Z6" t="n">
-        <v>-0.07450317809102414</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>0</v>
+    <row r="6" customFormat="1" s="5">
+      <c r="C6" s="5" t="n">
+        <v>-1.443289932012704e-15</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>-1.443289932012704e-15</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>-1.443289932012704e-15</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>-1.443289932012704e-15</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>-1.443289932012704e-15</v>
+      </c>
+      <c r="H6" s="5" t="n">
+        <v>-1.443289932012704e-15</v>
+      </c>
+      <c r="I6" s="5" t="n">
+        <v>-1.443289932012704e-15</v>
+      </c>
+      <c r="J6" s="5" t="n">
+        <v>-1.554312234475219e-15</v>
+      </c>
+      <c r="K6" s="5" t="n">
+        <v>0.2306768871614431</v>
       </c>
     </row>
-    <row r="7" customFormat="1" s="6">
-      <c r="A7" s="6" t="inlineStr">
+    <row r="7" customFormat="1" s="4">
+      <c r="A7" s="4" t="inlineStr">
         <is>
           <t>EFC</t>
         </is>
       </c>
-      <c r="B7" s="6" t="n">
+      <c r="B7" t="n">
         <v>775826.9428571428</v>
       </c>
       <c r="C7" t="n">
-        <v>888076.7000000001</v>
+        <v>775837.3999999999</v>
       </c>
       <c r="D7" t="n">
-        <v>228242.6857142857</v>
+        <v>775837.3999999999</v>
       </c>
       <c r="E7" t="n">
-        <v>1760370.871428571</v>
+        <v>775837.3999999999</v>
       </c>
       <c r="F7" t="n">
-        <v>939222.7428571428</v>
+        <v>775837.3999999999</v>
       </c>
       <c r="G7" t="n">
-        <v>1075381.285714286</v>
+        <v>775837.3999999999</v>
       </c>
       <c r="H7" t="n">
-        <v>1190594.242857143</v>
+        <v>775789.8428571429</v>
       </c>
       <c r="I7" t="n">
-        <v>1289344.757142857</v>
+        <v>773858.2714285713</v>
       </c>
       <c r="J7" t="n">
-        <v>779826.5999999999</v>
+        <v>705172.6142857142</v>
       </c>
       <c r="K7" t="n">
-        <v>783152.7857142857</v>
-      </c>
-      <c r="L7" t="n">
-        <v>785961.0857142856</v>
-      </c>
-      <c r="M7" t="n">
-        <v>788322.7428571428</v>
-      </c>
-      <c r="N7" t="n">
-        <v>780028.9285714286</v>
-      </c>
-      <c r="O7" t="n">
-        <v>783505.0285714285</v>
-      </c>
-      <c r="P7" t="n">
-        <v>786503.7857142857</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>786503.7857142857</v>
-      </c>
-      <c r="R7" t="n">
-        <v>275014.4142857143</v>
-      </c>
-      <c r="S7" t="n">
-        <v>620143.7857142857</v>
-      </c>
-      <c r="T7" t="n">
-        <v>448974.8428571429</v>
-      </c>
-      <c r="U7" t="n">
-        <v>768302.9428571428</v>
-      </c>
-      <c r="V7" t="n">
-        <v>774084.5857142857</v>
-      </c>
-      <c r="W7" t="n">
-        <v>771854.6142857142</v>
-      </c>
-      <c r="X7" t="n">
-        <v>714413.2571428572</v>
-      </c>
-      <c r="Y7" t="n">
-        <v>761317.8428571428</v>
-      </c>
-      <c r="Z7" t="n">
-        <v>744336.1428571427</v>
-      </c>
-      <c r="AA7" t="n">
-        <v>775826.9428571428</v>
-      </c>
-      <c r="AB7" t="n">
-        <v>775826.9428571428</v>
-      </c>
-      <c r="AC7" t="n">
-        <v>775826.9428571428</v>
-      </c>
-      <c r="AD7" t="n">
-        <v>775826.9428571428</v>
+        <v>74528.57142857142</v>
       </c>
     </row>
-    <row r="8" customFormat="1" s="3">
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="n">
-        <v>0.1446840151354816</v>
-      </c>
-      <c r="D8" t="n">
-        <v>-0.7058072192314758</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1.269025183561739</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.2106085661297883</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.386109744724735</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.5346131683343374</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.661897371589828</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.005155347052175685</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.009442624962422652</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0.01306237550841138</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.01610642697452813</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0.005416137906749219</v>
-      </c>
-      <c r="O8" t="n">
-        <v>0.009896647422438898</v>
-      </c>
-      <c r="P8" t="n">
-        <v>0.01376188717785864</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>0.01376188717785864</v>
-      </c>
-      <c r="R8" t="n">
-        <v>-0.6455209285811641</v>
-      </c>
-      <c r="S8" t="n">
-        <v>-0.200667376373295</v>
-      </c>
-      <c r="T8" t="n">
-        <v>-0.4212951135678527</v>
-      </c>
-      <c r="U8" t="n">
-        <v>-0.009698039065634045</v>
-      </c>
-      <c r="V8" t="n">
-        <v>-0.002245806437761066</v>
-      </c>
-      <c r="W8" t="n">
-        <v>-0.00512012196534406</v>
-      </c>
-      <c r="X8" t="n">
-        <v>-0.07915900095982364</v>
-      </c>
-      <c r="Y8" t="n">
-        <v>-0.01870146446134913</v>
-      </c>
-      <c r="Z8" t="n">
-        <v>-0.04058997987879709</v>
-      </c>
-      <c r="AA8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD8" t="n">
-        <v>0</v>
+    <row r="8" customFormat="1" s="5">
+      <c r="C8" s="5" t="n">
+        <v>1.347870546819507e-05</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>1.347870546819507e-05</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <v>1.347870546819507e-05</v>
+      </c>
+      <c r="F8" s="5" t="n">
+        <v>1.347870546819507e-05</v>
+      </c>
+      <c r="G8" s="5" t="n">
+        <v>1.347870546819507e-05</v>
+      </c>
+      <c r="H8" s="5" t="n">
+        <v>-4.78199427610404e-05</v>
+      </c>
+      <c r="I8" s="5" t="n">
+        <v>-0.002537513612663966</v>
+      </c>
+      <c r="J8" s="5" t="n">
+        <v>-0.09106970210551002</v>
+      </c>
+      <c r="K8" s="5" t="n">
+        <v>-0.9039366032402735</v>
       </c>
     </row>
     <row r="9">
@@ -1104,419 +684,140 @@
           <t>Leistungsflexibilität</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
     </row>
-    <row r="10" customFormat="1" s="5">
-      <c r="A10" s="5" t="inlineStr">
+    <row r="10" customFormat="1" s="3">
+      <c r="A10" s="3" t="inlineStr">
         <is>
           <t>APFI</t>
         </is>
       </c>
-      <c r="B10" s="5" t="n">
+      <c r="B10" t="n">
         <v>0.9168099390342248</v>
       </c>
       <c r="C10" t="n">
-        <v>0.9168099390342248</v>
+        <v>0.9075665989269164</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9332467158191154</v>
+        <v>0.896012423792781</v>
       </c>
       <c r="E10" t="n">
-        <v>0.8885039315660029</v>
+        <v>0.8811570557631783</v>
       </c>
       <c r="F10" t="n">
-        <v>0.9186184186204374</v>
+        <v>0.8613498983903747</v>
       </c>
       <c r="G10" t="n">
-        <v>0.9203499416285132</v>
+        <v>0.8336198780684496</v>
       </c>
       <c r="H10" t="n">
-        <v>0.9220093178445856</v>
+        <v>0.792024847585562</v>
       </c>
       <c r="I10" t="n">
-        <v>0.923600964419186</v>
+        <v>0.7226997967807494</v>
       </c>
       <c r="J10" t="n">
-        <v>0.9181824770017341</v>
+        <v>0.5840496951711238</v>
       </c>
       <c r="K10" t="n">
-        <v>0.9195104595630464</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0.9207960216069296</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0.9220061318205416</v>
-      </c>
-      <c r="N10" t="n">
-        <v>0.921592940486056</v>
-      </c>
-      <c r="O10" t="n">
-        <v>0.9258558485761345</v>
-      </c>
-      <c r="P10" t="n">
-        <v>0.9296791197361128</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>0.9331274291010668</v>
-      </c>
-      <c r="R10" t="n">
-        <v>0.9360492562162503</v>
-      </c>
-      <c r="S10" t="n">
-        <v>0.9202901284600205</v>
-      </c>
-      <c r="T10" t="n">
-        <v>0.9276992201971532</v>
-      </c>
-      <c r="U10" t="n">
-        <v>0.9105359304776882</v>
-      </c>
-      <c r="V10" t="n">
-        <v>0.9104638927538948</v>
-      </c>
-      <c r="W10" t="n">
-        <v>0.9096220584495044</v>
-      </c>
-      <c r="X10" t="n">
-        <v>0.860804624734176</v>
-      </c>
-      <c r="Y10" t="n">
-        <v>0.8722753858775544</v>
-      </c>
-      <c r="Z10" t="n">
-        <v>0.8628994366485037</v>
-      </c>
-      <c r="AA10" t="n">
-        <v>0.9168099390342248</v>
-      </c>
-      <c r="AB10" t="n">
-        <v>0.9168099390342248</v>
-      </c>
-      <c r="AC10" t="n">
-        <v>0.9168099390342248</v>
-      </c>
-      <c r="AD10" t="n">
-        <v>0.9168099390342248</v>
+        <v>0.3035901124213397</v>
       </c>
     </row>
-    <row r="11" customFormat="1" s="3">
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.01792822708947206</v>
-      </c>
-      <c r="E11" t="n">
-        <v>-0.03087445528572652</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.001972578512966061</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.003861217514741888</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.005671163224776787</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0.007407233599708851</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0.001497080157044417</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0.002945562012194536</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0.004347774171060692</v>
-      </c>
-      <c r="M11" t="n">
-        <v>0.005667688105334578</v>
-      </c>
-      <c r="N11" t="n">
-        <v>0.005217004362834121</v>
-      </c>
-      <c r="O11" t="n">
-        <v>0.0098667228143694</v>
-      </c>
-      <c r="P11" t="n">
-        <v>0.014036912291161</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>0.01779811646024587</v>
-      </c>
-      <c r="R11" t="n">
-        <v>0.02098506611118589</v>
-      </c>
-      <c r="S11" t="n">
-        <v>0.003795976982384985</v>
-      </c>
-      <c r="T11" t="n">
-        <v>0.01187735941693568</v>
-      </c>
-      <c r="U11" t="n">
-        <v>-0.006843303382100818</v>
-      </c>
-      <c r="V11" t="n">
-        <v>-0.006921877708933821</v>
-      </c>
-      <c r="W11" t="n">
-        <v>-0.00784009888929893</v>
-      </c>
-      <c r="X11" t="n">
-        <v>-0.06108715876165705</v>
-      </c>
-      <c r="Y11" t="n">
-        <v>-0.04857555667817426</v>
-      </c>
-      <c r="Z11" t="n">
-        <v>-0.05880226652266762</v>
-      </c>
-      <c r="AA11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD11" t="n">
-        <v>0</v>
+    <row r="11" customFormat="1" s="5">
+      <c r="C11" s="5" t="n">
+        <v>-0.0100820679551592</v>
+      </c>
+      <c r="D11" s="5" t="n">
+        <v>-0.02268465289910804</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <v>-0.03888797639847097</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <v>-0.06049240773095477</v>
+      </c>
+      <c r="G11" s="5" t="n">
+        <v>-0.09073861159643215</v>
+      </c>
+      <c r="H11" s="5" t="n">
+        <v>-0.1361079173946482</v>
+      </c>
+      <c r="I11" s="5" t="n">
+        <v>-0.2117234270583418</v>
+      </c>
+      <c r="J11" s="5" t="n">
+        <v>-0.3629544463857289</v>
+      </c>
+      <c r="K11" s="5" t="n">
+        <v>-0.6688625422831431</v>
       </c>
     </row>
-    <row r="12" customFormat="1" s="5">
-      <c r="A12" s="5" t="inlineStr">
+    <row r="12" customFormat="1" s="3">
+      <c r="A12" s="3" t="inlineStr">
         <is>
           <t>MPFI</t>
         </is>
       </c>
-      <c r="B12" s="5" t="n">
+      <c r="B12" t="n">
         <v>0.7429993474573815</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7429993474573814</v>
+        <v>0.7144437193970905</v>
       </c>
       <c r="D12" t="n">
-        <v>0.7281239317761206</v>
+        <v>0.6787491843217268</v>
       </c>
       <c r="E12" t="n">
-        <v>0.696499929658202</v>
+        <v>0.6328562106534019</v>
       </c>
       <c r="F12" t="n">
-        <v>0.742654623962453</v>
+        <v>0.5716655790956358</v>
       </c>
       <c r="G12" t="n">
-        <v>0.7454948450123886</v>
+        <v>0.4859986949147628</v>
       </c>
       <c r="H12" t="n">
-        <v>0.7466289143380886</v>
+        <v>0.3693447738722115</v>
       </c>
       <c r="I12" t="n">
-        <v>0.7478764746857323</v>
+        <v>0.2684656344681534</v>
       </c>
       <c r="J12" t="n">
-        <v>0.747999399400793</v>
+        <v>0.2118055947451971</v>
       </c>
       <c r="K12" t="n">
-        <v>0.7521477654169408</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0.7557639902517115</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0.7591482897592836</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0.7477920355825829</v>
-      </c>
-      <c r="O12" t="n">
-        <v>0.7502618293015826</v>
-      </c>
-      <c r="P12" t="n">
-        <v>0.7530085419819909</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>0.7651202071737672</v>
-      </c>
-      <c r="R12" t="n">
-        <v>0.7325114225101206</v>
-      </c>
-      <c r="S12" t="n">
-        <v>0.7293033265627984</v>
-      </c>
-      <c r="T12" t="n">
-        <v>0.7194730923381298</v>
-      </c>
-      <c r="U12" t="n">
-        <v>0.6967524434008689</v>
-      </c>
-      <c r="V12" t="n">
-        <v>0.7171143896473335</v>
-      </c>
-      <c r="W12" t="n">
-        <v>0.707287097972551</v>
-      </c>
-      <c r="X12" t="n">
-        <v>0.6486677321224686</v>
-      </c>
-      <c r="Y12" t="n">
-        <v>0.6510811268107422</v>
-      </c>
-      <c r="Z12" t="n">
-        <v>0.6366296351385665</v>
-      </c>
-      <c r="AA12" t="n">
-        <v>0.7429993474573815</v>
-      </c>
-      <c r="AB12" t="n">
-        <v>0.7429993474573815</v>
-      </c>
-      <c r="AC12" t="n">
-        <v>0.7429993474573815</v>
-      </c>
-      <c r="AD12" t="n">
-        <v>0.7429993474573815</v>
+        <v>0.1574074074074074</v>
       </c>
     </row>
-    <row r="13" customFormat="1" s="4">
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="n">
-        <v>-1.110223024625157e-16</v>
-      </c>
-      <c r="D13" t="n">
-        <v>-0.02002076547195653</v>
-      </c>
-      <c r="E13" t="n">
-        <v>-0.06258338982168055</v>
-      </c>
-      <c r="F13" t="n">
-        <v>-0.0004639620426427626</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.003358680681950776</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0.004885020280472441</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0.006564107014414899</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0.006729550921575012</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0.01231282098815578</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0.01717988425967243</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0.02173480011411244</v>
-      </c>
-      <c r="N13" t="n">
-        <v>0.006450460746166842</v>
-      </c>
-      <c r="O13" t="n">
-        <v>0.009774546732852496</v>
-      </c>
-      <c r="P13" t="n">
-        <v>0.0134713368980226</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>0.02977238108227875</v>
-      </c>
-      <c r="R13" t="n">
-        <v>-0.0141156583557599</v>
-      </c>
-      <c r="S13" t="n">
-        <v>-0.01843342250764046</v>
-      </c>
-      <c r="T13" t="n">
-        <v>-0.03166389741762343</v>
-      </c>
-      <c r="U13" t="n">
-        <v>-0.06224353253441484</v>
-      </c>
-      <c r="V13" t="n">
-        <v>-0.03483846641134869</v>
-      </c>
-      <c r="W13" t="n">
-        <v>-0.0480649809546152</v>
-      </c>
-      <c r="X13" t="n">
-        <v>-0.1269605628291938</v>
-      </c>
-      <c r="Y13" t="n">
-        <v>-0.1237123840837717</v>
-      </c>
-      <c r="Z13" t="n">
-        <v>-0.1431625918418675</v>
-      </c>
-      <c r="AA13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD13" t="n">
-        <v>0</v>
+    <row r="13" customFormat="1" s="5">
+      <c r="C13" s="5" t="n">
+        <v>-0.03843291135855131</v>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>-0.08647405055674029</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>-0.1482412295258407</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>-0.2305974681513074</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>-0.3458962022269613</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>-0.5029002715330149</v>
+      </c>
+      <c r="I13" s="5" t="n">
+        <v>-0.6386731221408608</v>
+      </c>
+      <c r="J13" s="5" t="n">
+        <v>-0.7149316544220164</v>
+      </c>
+      <c r="K13" s="5" t="n">
+        <v>-0.7881459681679783</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:XFD5">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A6:XFD6">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A7:XFD7">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8:XFD8">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -1542,9 +843,585 @@
           <t>Base</t>
         </is>
       </c>
+      <c r="B1" t="inlineStr"/>
+      <c r="C1" t="inlineStr"/>
+      <c r="D1" t="inlineStr"/>
+      <c r="E1" t="inlineStr"/>
+      <c r="F1" t="inlineStr"/>
+      <c r="G1" t="inlineStr"/>
+      <c r="H1" t="inlineStr"/>
+      <c r="I1" t="inlineStr"/>
+      <c r="J1" t="inlineStr"/>
+      <c r="K1" t="inlineStr"/>
+      <c r="L1" t="inlineStr"/>
+      <c r="M1" t="inlineStr"/>
+      <c r="N1" t="inlineStr"/>
+      <c r="O1" t="inlineStr"/>
+      <c r="P1" t="inlineStr"/>
+      <c r="Q1" t="inlineStr"/>
+      <c r="R1" t="inlineStr"/>
+      <c r="S1" t="inlineStr"/>
+      <c r="T1" t="inlineStr"/>
+      <c r="U1" t="inlineStr"/>
+      <c r="V1" t="inlineStr"/>
+      <c r="W1" t="inlineStr"/>
+      <c r="X1" t="inlineStr"/>
+      <c r="Y1" t="inlineStr"/>
+      <c r="Z1" t="inlineStr"/>
+      <c r="AA1" t="inlineStr"/>
+      <c r="AB1" t="inlineStr"/>
+      <c r="AC1" t="inlineStr"/>
+      <c r="AD1" t="inlineStr"/>
+      <c r="AE1" t="inlineStr"/>
+      <c r="AF1" t="inlineStr"/>
+      <c r="AG1" t="inlineStr"/>
+      <c r="AH1" t="inlineStr"/>
+      <c r="AI1" t="inlineStr"/>
+      <c r="AJ1" t="inlineStr"/>
+      <c r="AK1" t="inlineStr"/>
+      <c r="AL1" t="inlineStr"/>
+      <c r="AM1" t="inlineStr"/>
+      <c r="AN1" t="inlineStr"/>
+      <c r="AO1" t="inlineStr"/>
+      <c r="AP1" t="inlineStr"/>
+      <c r="AQ1" t="inlineStr"/>
+      <c r="AR1" t="inlineStr"/>
+      <c r="AS1" t="inlineStr"/>
+      <c r="AT1" t="inlineStr"/>
+      <c r="AU1" t="inlineStr"/>
+      <c r="AV1" t="inlineStr"/>
+      <c r="AW1" t="inlineStr"/>
+      <c r="AX1" t="inlineStr"/>
+      <c r="AY1" t="inlineStr"/>
+      <c r="AZ1" t="inlineStr"/>
+      <c r="BA1" t="inlineStr"/>
+      <c r="BB1" t="inlineStr"/>
+      <c r="BC1" t="inlineStr"/>
+      <c r="BD1" t="inlineStr"/>
+      <c r="BE1" t="inlineStr"/>
+      <c r="BF1" t="inlineStr"/>
+      <c r="BG1" t="inlineStr"/>
+      <c r="BH1" t="inlineStr"/>
+      <c r="BI1" t="inlineStr"/>
+      <c r="BJ1" t="inlineStr"/>
+      <c r="BK1" t="inlineStr"/>
+      <c r="BL1" t="inlineStr"/>
+      <c r="BM1" t="inlineStr"/>
+      <c r="BN1" t="inlineStr"/>
+      <c r="BO1" t="inlineStr"/>
+      <c r="BP1" t="inlineStr"/>
+      <c r="BQ1" t="inlineStr"/>
+      <c r="BR1" t="inlineStr"/>
+      <c r="BS1" t="inlineStr"/>
+      <c r="BT1" t="inlineStr"/>
+      <c r="BU1" t="inlineStr"/>
+      <c r="BV1" t="inlineStr"/>
+      <c r="BW1" t="inlineStr"/>
+      <c r="BX1" t="inlineStr"/>
+      <c r="BY1" t="inlineStr"/>
+      <c r="BZ1" t="inlineStr"/>
+      <c r="CA1" t="inlineStr"/>
+      <c r="CB1" t="inlineStr"/>
+      <c r="CC1" t="inlineStr"/>
+      <c r="CD1" t="inlineStr"/>
+      <c r="CE1" t="inlineStr"/>
+      <c r="CF1" t="inlineStr"/>
+      <c r="CG1" t="inlineStr"/>
+      <c r="CH1" t="inlineStr"/>
+      <c r="CI1" t="inlineStr"/>
+      <c r="CJ1" t="inlineStr"/>
+      <c r="CK1" t="inlineStr"/>
+      <c r="CL1" t="inlineStr"/>
+      <c r="CM1" t="inlineStr"/>
+      <c r="CN1" t="inlineStr"/>
+      <c r="CO1" t="inlineStr"/>
+      <c r="CP1" t="inlineStr"/>
+      <c r="CQ1" t="inlineStr"/>
+      <c r="CR1" t="inlineStr"/>
+      <c r="CS1" t="inlineStr"/>
+      <c r="CT1" t="inlineStr"/>
+      <c r="CU1" t="inlineStr"/>
+      <c r="CV1" t="inlineStr"/>
+      <c r="CW1" t="inlineStr"/>
+      <c r="CX1" t="inlineStr"/>
+      <c r="CY1" t="inlineStr"/>
+      <c r="CZ1" t="inlineStr"/>
+      <c r="DA1" t="inlineStr"/>
+      <c r="DB1" t="inlineStr"/>
+      <c r="DC1" t="inlineStr"/>
+      <c r="DD1" t="inlineStr"/>
+      <c r="DE1" t="inlineStr"/>
+      <c r="DF1" t="inlineStr"/>
+      <c r="DG1" t="inlineStr"/>
+      <c r="DH1" t="inlineStr"/>
+      <c r="DI1" t="inlineStr"/>
+      <c r="DJ1" t="inlineStr"/>
+      <c r="DK1" t="inlineStr"/>
+      <c r="DL1" t="inlineStr"/>
+      <c r="DM1" t="inlineStr"/>
+      <c r="DN1" t="inlineStr"/>
+      <c r="DO1" t="inlineStr"/>
+      <c r="DP1" t="inlineStr"/>
+      <c r="DQ1" t="inlineStr"/>
+      <c r="DR1" t="inlineStr"/>
+      <c r="DS1" t="inlineStr"/>
+      <c r="DT1" t="inlineStr"/>
+      <c r="DU1" t="inlineStr"/>
+      <c r="DV1" t="inlineStr"/>
+      <c r="DW1" t="inlineStr"/>
+      <c r="DX1" t="inlineStr"/>
+      <c r="DY1" t="inlineStr"/>
+      <c r="DZ1" t="inlineStr"/>
+      <c r="EA1" t="inlineStr"/>
+      <c r="EB1" t="inlineStr"/>
+      <c r="EC1" t="inlineStr"/>
+      <c r="ED1" t="inlineStr"/>
+      <c r="EE1" t="inlineStr"/>
+      <c r="EF1" t="inlineStr"/>
+      <c r="EG1" t="inlineStr"/>
+      <c r="EH1" t="inlineStr"/>
+      <c r="EI1" t="inlineStr"/>
+      <c r="EJ1" t="inlineStr"/>
+      <c r="EK1" t="inlineStr"/>
+      <c r="EL1" t="inlineStr"/>
+      <c r="EM1" t="inlineStr"/>
+      <c r="EN1" t="inlineStr"/>
+      <c r="EO1" t="inlineStr"/>
+      <c r="EP1" t="inlineStr"/>
+      <c r="EQ1" t="inlineStr"/>
+      <c r="ER1" t="inlineStr"/>
+      <c r="ES1" t="inlineStr"/>
+      <c r="ET1" t="inlineStr"/>
+      <c r="EU1" t="inlineStr"/>
+      <c r="EV1" t="inlineStr"/>
+      <c r="EW1" t="inlineStr"/>
+      <c r="EX1" t="inlineStr"/>
+      <c r="EY1" t="inlineStr"/>
+      <c r="EZ1" t="inlineStr"/>
+      <c r="FA1" t="inlineStr"/>
+      <c r="FB1" t="inlineStr"/>
+      <c r="FC1" t="inlineStr"/>
+      <c r="FD1" t="inlineStr"/>
+      <c r="FE1" t="inlineStr"/>
+      <c r="FF1" t="inlineStr"/>
+      <c r="FG1" t="inlineStr"/>
+      <c r="FH1" t="inlineStr"/>
+      <c r="FI1" t="inlineStr"/>
+      <c r="FJ1" t="inlineStr"/>
+      <c r="FK1" t="inlineStr"/>
+      <c r="FL1" t="inlineStr"/>
+      <c r="FM1" t="inlineStr"/>
+      <c r="FN1" t="inlineStr"/>
+      <c r="FO1" t="inlineStr"/>
+      <c r="FP1" t="inlineStr"/>
+      <c r="FQ1" t="inlineStr"/>
+      <c r="FR1" t="inlineStr"/>
+      <c r="FS1" t="inlineStr"/>
+      <c r="FT1" t="inlineStr"/>
+      <c r="FU1" t="inlineStr"/>
+      <c r="FV1" t="inlineStr"/>
+      <c r="FW1" t="inlineStr"/>
+      <c r="FX1" t="inlineStr"/>
+      <c r="FY1" t="inlineStr"/>
+      <c r="FZ1" t="inlineStr"/>
+      <c r="GA1" t="inlineStr"/>
+      <c r="GB1" t="inlineStr"/>
+      <c r="GC1" t="inlineStr"/>
+      <c r="GD1" t="inlineStr"/>
+      <c r="GE1" t="inlineStr"/>
+      <c r="GF1" t="inlineStr"/>
+      <c r="GG1" t="inlineStr"/>
+      <c r="GH1" t="inlineStr"/>
+      <c r="GI1" t="inlineStr"/>
+      <c r="GJ1" t="inlineStr"/>
+      <c r="GK1" t="inlineStr"/>
+      <c r="GL1" t="inlineStr"/>
+      <c r="GM1" t="inlineStr"/>
+      <c r="GN1" t="inlineStr"/>
+      <c r="GO1" t="inlineStr"/>
+      <c r="GP1" t="inlineStr"/>
+      <c r="GQ1" t="inlineStr"/>
+      <c r="GR1" t="inlineStr"/>
+      <c r="GS1" t="inlineStr"/>
+      <c r="GT1" t="inlineStr"/>
+      <c r="GU1" t="inlineStr"/>
+      <c r="GV1" t="inlineStr"/>
+      <c r="GW1" t="inlineStr"/>
+      <c r="GX1" t="inlineStr"/>
+      <c r="GY1" t="inlineStr"/>
+      <c r="GZ1" t="inlineStr"/>
+      <c r="HA1" t="inlineStr"/>
+      <c r="HB1" t="inlineStr"/>
+      <c r="HC1" t="inlineStr"/>
+      <c r="HD1" t="inlineStr"/>
+      <c r="HE1" t="inlineStr"/>
+      <c r="HF1" t="inlineStr"/>
+      <c r="HG1" t="inlineStr"/>
+      <c r="HH1" t="inlineStr"/>
+      <c r="HI1" t="inlineStr"/>
+      <c r="HJ1" t="inlineStr"/>
+      <c r="HK1" t="inlineStr"/>
+      <c r="HL1" t="inlineStr"/>
+      <c r="HM1" t="inlineStr"/>
+      <c r="HN1" t="inlineStr"/>
+      <c r="HO1" t="inlineStr"/>
+      <c r="HP1" t="inlineStr"/>
+      <c r="HQ1" t="inlineStr"/>
+      <c r="HR1" t="inlineStr"/>
+      <c r="HS1" t="inlineStr"/>
+      <c r="HT1" t="inlineStr"/>
+      <c r="HU1" t="inlineStr"/>
+      <c r="HV1" t="inlineStr"/>
+      <c r="HW1" t="inlineStr"/>
+      <c r="HX1" t="inlineStr"/>
+      <c r="HY1" t="inlineStr"/>
+      <c r="HZ1" t="inlineStr"/>
+      <c r="IA1" t="inlineStr"/>
+      <c r="IB1" t="inlineStr"/>
+      <c r="IC1" t="inlineStr"/>
+      <c r="ID1" t="inlineStr"/>
+      <c r="IE1" t="inlineStr"/>
+      <c r="IF1" t="inlineStr"/>
+      <c r="IG1" t="inlineStr"/>
+      <c r="IH1" t="inlineStr"/>
+      <c r="II1" t="inlineStr"/>
+      <c r="IJ1" t="inlineStr"/>
+      <c r="IK1" t="inlineStr"/>
+      <c r="IL1" t="inlineStr"/>
+      <c r="IM1" t="inlineStr"/>
+      <c r="IN1" t="inlineStr"/>
+      <c r="IO1" t="inlineStr"/>
+      <c r="IP1" t="inlineStr"/>
+      <c r="IQ1" t="inlineStr"/>
+      <c r="IR1" t="inlineStr"/>
+      <c r="IS1" t="inlineStr"/>
+      <c r="IT1" t="inlineStr"/>
+      <c r="IU1" t="inlineStr"/>
+      <c r="IV1" t="inlineStr"/>
+      <c r="IW1" t="inlineStr"/>
+      <c r="IX1" t="inlineStr"/>
+      <c r="IY1" t="inlineStr"/>
+      <c r="IZ1" t="inlineStr"/>
+      <c r="JA1" t="inlineStr"/>
+      <c r="JB1" t="inlineStr"/>
+      <c r="JC1" t="inlineStr"/>
+      <c r="JD1" t="inlineStr"/>
+      <c r="JE1" t="inlineStr"/>
+      <c r="JF1" t="inlineStr"/>
+      <c r="JG1" t="inlineStr"/>
+      <c r="JH1" t="inlineStr"/>
+      <c r="JI1" t="inlineStr"/>
+      <c r="JJ1" t="inlineStr"/>
+      <c r="JK1" t="inlineStr"/>
+      <c r="JL1" t="inlineStr"/>
+      <c r="JM1" t="inlineStr"/>
+      <c r="JN1" t="inlineStr"/>
+      <c r="JO1" t="inlineStr"/>
+      <c r="JP1" t="inlineStr"/>
+      <c r="JQ1" t="inlineStr"/>
+      <c r="JR1" t="inlineStr"/>
+      <c r="JS1" t="inlineStr"/>
+      <c r="JT1" t="inlineStr"/>
+      <c r="JU1" t="inlineStr"/>
+      <c r="JV1" t="inlineStr"/>
+      <c r="JW1" t="inlineStr"/>
+      <c r="JX1" t="inlineStr"/>
+      <c r="JY1" t="inlineStr"/>
+      <c r="JZ1" t="inlineStr"/>
+      <c r="KA1" t="inlineStr"/>
+      <c r="KB1" t="inlineStr"/>
+      <c r="KC1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="inlineStr"/>
+      <c r="AJ2" t="inlineStr"/>
+      <c r="AK2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr"/>
+      <c r="AM2" t="inlineStr"/>
+      <c r="AN2" t="inlineStr"/>
+      <c r="AO2" t="inlineStr"/>
+      <c r="AP2" t="inlineStr"/>
+      <c r="AQ2" t="inlineStr"/>
+      <c r="AR2" t="inlineStr"/>
+      <c r="AS2" t="inlineStr"/>
+      <c r="AT2" t="inlineStr"/>
+      <c r="AU2" t="inlineStr"/>
+      <c r="AV2" t="inlineStr"/>
+      <c r="AW2" t="inlineStr"/>
+      <c r="AX2" t="inlineStr"/>
+      <c r="AY2" t="inlineStr"/>
+      <c r="AZ2" t="inlineStr"/>
+      <c r="BA2" t="inlineStr"/>
+      <c r="BB2" t="inlineStr"/>
+      <c r="BC2" t="inlineStr"/>
+      <c r="BD2" t="inlineStr"/>
+      <c r="BE2" t="inlineStr"/>
+      <c r="BF2" t="inlineStr"/>
+      <c r="BG2" t="inlineStr"/>
+      <c r="BH2" t="inlineStr"/>
+      <c r="BI2" t="inlineStr"/>
+      <c r="BJ2" t="inlineStr"/>
+      <c r="BK2" t="inlineStr"/>
+      <c r="BL2" t="inlineStr"/>
+      <c r="BM2" t="inlineStr"/>
+      <c r="BN2" t="inlineStr"/>
+      <c r="BO2" t="inlineStr"/>
+      <c r="BP2" t="inlineStr"/>
+      <c r="BQ2" t="inlineStr"/>
+      <c r="BR2" t="inlineStr"/>
+      <c r="BS2" t="inlineStr"/>
+      <c r="BT2" t="inlineStr"/>
+      <c r="BU2" t="inlineStr"/>
+      <c r="BV2" t="inlineStr"/>
+      <c r="BW2" t="inlineStr"/>
+      <c r="BX2" t="inlineStr"/>
+      <c r="BY2" t="inlineStr"/>
+      <c r="BZ2" t="inlineStr"/>
+      <c r="CA2" t="inlineStr"/>
+      <c r="CB2" t="inlineStr"/>
+      <c r="CC2" t="inlineStr"/>
+      <c r="CD2" t="inlineStr"/>
+      <c r="CE2" t="inlineStr"/>
+      <c r="CF2" t="inlineStr"/>
+      <c r="CG2" t="inlineStr"/>
+      <c r="CH2" t="inlineStr"/>
+      <c r="CI2" t="inlineStr"/>
+      <c r="CJ2" t="inlineStr"/>
+      <c r="CK2" t="inlineStr"/>
+      <c r="CL2" t="inlineStr"/>
+      <c r="CM2" t="inlineStr"/>
+      <c r="CN2" t="inlineStr"/>
+      <c r="CO2" t="inlineStr"/>
+      <c r="CP2" t="inlineStr"/>
+      <c r="CQ2" t="inlineStr"/>
+      <c r="CR2" t="inlineStr"/>
+      <c r="CS2" t="inlineStr"/>
+      <c r="CT2" t="inlineStr"/>
+      <c r="CU2" t="inlineStr"/>
+      <c r="CV2" t="inlineStr"/>
+      <c r="CW2" t="inlineStr"/>
+      <c r="CX2" t="inlineStr"/>
+      <c r="CY2" t="inlineStr"/>
+      <c r="CZ2" t="inlineStr"/>
+      <c r="DA2" t="inlineStr"/>
+      <c r="DB2" t="inlineStr"/>
+      <c r="DC2" t="inlineStr"/>
+      <c r="DD2" t="inlineStr"/>
+      <c r="DE2" t="inlineStr"/>
+      <c r="DF2" t="inlineStr"/>
+      <c r="DG2" t="inlineStr"/>
+      <c r="DH2" t="inlineStr"/>
+      <c r="DI2" t="inlineStr"/>
+      <c r="DJ2" t="inlineStr"/>
+      <c r="DK2" t="inlineStr"/>
+      <c r="DL2" t="inlineStr"/>
+      <c r="DM2" t="inlineStr"/>
+      <c r="DN2" t="inlineStr"/>
+      <c r="DO2" t="inlineStr"/>
+      <c r="DP2" t="inlineStr"/>
+      <c r="DQ2" t="inlineStr"/>
+      <c r="DR2" t="inlineStr"/>
+      <c r="DS2" t="inlineStr"/>
+      <c r="DT2" t="inlineStr"/>
+      <c r="DU2" t="inlineStr"/>
+      <c r="DV2" t="inlineStr"/>
+      <c r="DW2" t="inlineStr"/>
+      <c r="DX2" t="inlineStr"/>
+      <c r="DY2" t="inlineStr"/>
+      <c r="DZ2" t="inlineStr"/>
+      <c r="EA2" t="inlineStr"/>
+      <c r="EB2" t="inlineStr"/>
+      <c r="EC2" t="inlineStr"/>
+      <c r="ED2" t="inlineStr"/>
+      <c r="EE2" t="inlineStr"/>
+      <c r="EF2" t="inlineStr"/>
+      <c r="EG2" t="inlineStr"/>
+      <c r="EH2" t="inlineStr"/>
+      <c r="EI2" t="inlineStr"/>
+      <c r="EJ2" t="inlineStr"/>
+      <c r="EK2" t="inlineStr"/>
+      <c r="EL2" t="inlineStr"/>
+      <c r="EM2" t="inlineStr"/>
+      <c r="EN2" t="inlineStr"/>
+      <c r="EO2" t="inlineStr"/>
+      <c r="EP2" t="inlineStr"/>
+      <c r="EQ2" t="inlineStr"/>
+      <c r="ER2" t="inlineStr"/>
+      <c r="ES2" t="inlineStr"/>
+      <c r="ET2" t="inlineStr"/>
+      <c r="EU2" t="inlineStr"/>
+      <c r="EV2" t="inlineStr"/>
+      <c r="EW2" t="inlineStr"/>
+      <c r="EX2" t="inlineStr"/>
+      <c r="EY2" t="inlineStr"/>
+      <c r="EZ2" t="inlineStr"/>
+      <c r="FA2" t="inlineStr"/>
+      <c r="FB2" t="inlineStr"/>
+      <c r="FC2" t="inlineStr"/>
+      <c r="FD2" t="inlineStr"/>
+      <c r="FE2" t="inlineStr"/>
+      <c r="FF2" t="inlineStr"/>
+      <c r="FG2" t="inlineStr"/>
+      <c r="FH2" t="inlineStr"/>
+      <c r="FI2" t="inlineStr"/>
+      <c r="FJ2" t="inlineStr"/>
+      <c r="FK2" t="inlineStr"/>
+      <c r="FL2" t="inlineStr"/>
+      <c r="FM2" t="inlineStr"/>
+      <c r="FN2" t="inlineStr"/>
+      <c r="FO2" t="inlineStr"/>
+      <c r="FP2" t="inlineStr"/>
+      <c r="FQ2" t="inlineStr"/>
+      <c r="FR2" t="inlineStr"/>
+      <c r="FS2" t="inlineStr"/>
+      <c r="FT2" t="inlineStr"/>
+      <c r="FU2" t="inlineStr"/>
+      <c r="FV2" t="inlineStr"/>
+      <c r="FW2" t="inlineStr"/>
+      <c r="FX2" t="inlineStr"/>
+      <c r="FY2" t="inlineStr"/>
+      <c r="FZ2" t="inlineStr"/>
+      <c r="GA2" t="inlineStr"/>
+      <c r="GB2" t="inlineStr"/>
+      <c r="GC2" t="inlineStr"/>
+      <c r="GD2" t="inlineStr"/>
+      <c r="GE2" t="inlineStr"/>
+      <c r="GF2" t="inlineStr"/>
+      <c r="GG2" t="inlineStr"/>
+      <c r="GH2" t="inlineStr"/>
+      <c r="GI2" t="inlineStr"/>
+      <c r="GJ2" t="inlineStr"/>
+      <c r="GK2" t="inlineStr"/>
+      <c r="GL2" t="inlineStr"/>
+      <c r="GM2" t="inlineStr"/>
+      <c r="GN2" t="inlineStr"/>
+      <c r="GO2" t="inlineStr"/>
+      <c r="GP2" t="inlineStr"/>
+      <c r="GQ2" t="inlineStr"/>
+      <c r="GR2" t="inlineStr"/>
+      <c r="GS2" t="inlineStr"/>
+      <c r="GT2" t="inlineStr"/>
+      <c r="GU2" t="inlineStr"/>
+      <c r="GV2" t="inlineStr"/>
+      <c r="GW2" t="inlineStr"/>
+      <c r="GX2" t="inlineStr"/>
+      <c r="GY2" t="inlineStr"/>
+      <c r="GZ2" t="inlineStr"/>
+      <c r="HA2" t="inlineStr"/>
+      <c r="HB2" t="inlineStr"/>
+      <c r="HC2" t="inlineStr"/>
+      <c r="HD2" t="inlineStr"/>
+      <c r="HE2" t="inlineStr"/>
+      <c r="HF2" t="inlineStr"/>
+      <c r="HG2" t="inlineStr"/>
+      <c r="HH2" t="inlineStr"/>
+      <c r="HI2" t="inlineStr"/>
+      <c r="HJ2" t="inlineStr"/>
+      <c r="HK2" t="inlineStr"/>
+      <c r="HL2" t="inlineStr"/>
+      <c r="HM2" t="inlineStr"/>
+      <c r="HN2" t="inlineStr"/>
+      <c r="HO2" t="inlineStr"/>
+      <c r="HP2" t="inlineStr"/>
+      <c r="HQ2" t="inlineStr"/>
+      <c r="HR2" t="inlineStr"/>
+      <c r="HS2" t="inlineStr"/>
+      <c r="HT2" t="inlineStr"/>
+      <c r="HU2" t="inlineStr"/>
+      <c r="HV2" t="inlineStr"/>
+      <c r="HW2" t="inlineStr"/>
+      <c r="HX2" t="inlineStr"/>
+      <c r="HY2" t="inlineStr"/>
+      <c r="HZ2" t="inlineStr"/>
+      <c r="IA2" t="inlineStr"/>
+      <c r="IB2" t="inlineStr"/>
+      <c r="IC2" t="inlineStr"/>
+      <c r="ID2" t="inlineStr"/>
+      <c r="IE2" t="inlineStr"/>
+      <c r="IF2" t="inlineStr"/>
+      <c r="IG2" t="inlineStr"/>
+      <c r="IH2" t="inlineStr"/>
+      <c r="II2" t="inlineStr"/>
+      <c r="IJ2" t="inlineStr"/>
+      <c r="IK2" t="inlineStr"/>
+      <c r="IL2" t="inlineStr"/>
+      <c r="IM2" t="inlineStr"/>
+      <c r="IN2" t="inlineStr"/>
+      <c r="IO2" t="inlineStr"/>
+      <c r="IP2" t="inlineStr"/>
+      <c r="IQ2" t="inlineStr"/>
+      <c r="IR2" t="inlineStr"/>
+      <c r="IS2" t="inlineStr"/>
+      <c r="IT2" t="inlineStr"/>
+      <c r="IU2" t="inlineStr"/>
+      <c r="IV2" t="inlineStr"/>
+      <c r="IW2" t="inlineStr"/>
+      <c r="IX2" t="inlineStr"/>
+      <c r="IY2" t="inlineStr"/>
+      <c r="IZ2" t="inlineStr"/>
+      <c r="JA2" t="inlineStr"/>
+      <c r="JB2" t="inlineStr"/>
+      <c r="JC2" t="inlineStr"/>
+      <c r="JD2" t="inlineStr"/>
+      <c r="JE2" t="inlineStr"/>
+      <c r="JF2" t="inlineStr"/>
+      <c r="JG2" t="inlineStr"/>
+      <c r="JH2" t="inlineStr"/>
+      <c r="JI2" t="inlineStr"/>
+      <c r="JJ2" t="inlineStr"/>
+      <c r="JK2" t="inlineStr"/>
+      <c r="JL2" t="inlineStr"/>
+      <c r="JM2" t="inlineStr"/>
+      <c r="JN2" t="inlineStr"/>
+      <c r="JO2" t="inlineStr"/>
+      <c r="JP2" t="inlineStr"/>
+      <c r="JQ2" t="inlineStr"/>
+      <c r="JR2" t="inlineStr"/>
+      <c r="JS2" t="inlineStr"/>
+      <c r="JT2" t="inlineStr"/>
+      <c r="JU2" t="inlineStr"/>
+      <c r="JV2" t="inlineStr"/>
+      <c r="JW2" t="inlineStr"/>
+      <c r="JX2" t="inlineStr"/>
+      <c r="JY2" t="inlineStr"/>
+      <c r="JZ2" t="inlineStr"/>
+      <c r="KA2" t="inlineStr"/>
+      <c r="KB2" t="inlineStr"/>
+      <c r="KC2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
@@ -2419,6 +2296,294 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="inlineStr"/>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="inlineStr"/>
+      <c r="AI4" t="inlineStr"/>
+      <c r="AJ4" t="inlineStr"/>
+      <c r="AK4" t="inlineStr"/>
+      <c r="AL4" t="inlineStr"/>
+      <c r="AM4" t="inlineStr"/>
+      <c r="AN4" t="inlineStr"/>
+      <c r="AO4" t="inlineStr"/>
+      <c r="AP4" t="inlineStr"/>
+      <c r="AQ4" t="inlineStr"/>
+      <c r="AR4" t="inlineStr"/>
+      <c r="AS4" t="inlineStr"/>
+      <c r="AT4" t="inlineStr"/>
+      <c r="AU4" t="inlineStr"/>
+      <c r="AV4" t="inlineStr"/>
+      <c r="AW4" t="inlineStr"/>
+      <c r="AX4" t="inlineStr"/>
+      <c r="AY4" t="inlineStr"/>
+      <c r="AZ4" t="inlineStr"/>
+      <c r="BA4" t="inlineStr"/>
+      <c r="BB4" t="inlineStr"/>
+      <c r="BC4" t="inlineStr"/>
+      <c r="BD4" t="inlineStr"/>
+      <c r="BE4" t="inlineStr"/>
+      <c r="BF4" t="inlineStr"/>
+      <c r="BG4" t="inlineStr"/>
+      <c r="BH4" t="inlineStr"/>
+      <c r="BI4" t="inlineStr"/>
+      <c r="BJ4" t="inlineStr"/>
+      <c r="BK4" t="inlineStr"/>
+      <c r="BL4" t="inlineStr"/>
+      <c r="BM4" t="inlineStr"/>
+      <c r="BN4" t="inlineStr"/>
+      <c r="BO4" t="inlineStr"/>
+      <c r="BP4" t="inlineStr"/>
+      <c r="BQ4" t="inlineStr"/>
+      <c r="BR4" t="inlineStr"/>
+      <c r="BS4" t="inlineStr"/>
+      <c r="BT4" t="inlineStr"/>
+      <c r="BU4" t="inlineStr"/>
+      <c r="BV4" t="inlineStr"/>
+      <c r="BW4" t="inlineStr"/>
+      <c r="BX4" t="inlineStr"/>
+      <c r="BY4" t="inlineStr"/>
+      <c r="BZ4" t="inlineStr"/>
+      <c r="CA4" t="inlineStr"/>
+      <c r="CB4" t="inlineStr"/>
+      <c r="CC4" t="inlineStr"/>
+      <c r="CD4" t="inlineStr"/>
+      <c r="CE4" t="inlineStr"/>
+      <c r="CF4" t="inlineStr"/>
+      <c r="CG4" t="inlineStr"/>
+      <c r="CH4" t="inlineStr"/>
+      <c r="CI4" t="inlineStr"/>
+      <c r="CJ4" t="inlineStr"/>
+      <c r="CK4" t="inlineStr"/>
+      <c r="CL4" t="inlineStr"/>
+      <c r="CM4" t="inlineStr"/>
+      <c r="CN4" t="inlineStr"/>
+      <c r="CO4" t="inlineStr"/>
+      <c r="CP4" t="inlineStr"/>
+      <c r="CQ4" t="inlineStr"/>
+      <c r="CR4" t="inlineStr"/>
+      <c r="CS4" t="inlineStr"/>
+      <c r="CT4" t="inlineStr"/>
+      <c r="CU4" t="inlineStr"/>
+      <c r="CV4" t="inlineStr"/>
+      <c r="CW4" t="inlineStr"/>
+      <c r="CX4" t="inlineStr"/>
+      <c r="CY4" t="inlineStr"/>
+      <c r="CZ4" t="inlineStr"/>
+      <c r="DA4" t="inlineStr"/>
+      <c r="DB4" t="inlineStr"/>
+      <c r="DC4" t="inlineStr"/>
+      <c r="DD4" t="inlineStr"/>
+      <c r="DE4" t="inlineStr"/>
+      <c r="DF4" t="inlineStr"/>
+      <c r="DG4" t="inlineStr"/>
+      <c r="DH4" t="inlineStr"/>
+      <c r="DI4" t="inlineStr"/>
+      <c r="DJ4" t="inlineStr"/>
+      <c r="DK4" t="inlineStr"/>
+      <c r="DL4" t="inlineStr"/>
+      <c r="DM4" t="inlineStr"/>
+      <c r="DN4" t="inlineStr"/>
+      <c r="DO4" t="inlineStr"/>
+      <c r="DP4" t="inlineStr"/>
+      <c r="DQ4" t="inlineStr"/>
+      <c r="DR4" t="inlineStr"/>
+      <c r="DS4" t="inlineStr"/>
+      <c r="DT4" t="inlineStr"/>
+      <c r="DU4" t="inlineStr"/>
+      <c r="DV4" t="inlineStr"/>
+      <c r="DW4" t="inlineStr"/>
+      <c r="DX4" t="inlineStr"/>
+      <c r="DY4" t="inlineStr"/>
+      <c r="DZ4" t="inlineStr"/>
+      <c r="EA4" t="inlineStr"/>
+      <c r="EB4" t="inlineStr"/>
+      <c r="EC4" t="inlineStr"/>
+      <c r="ED4" t="inlineStr"/>
+      <c r="EE4" t="inlineStr"/>
+      <c r="EF4" t="inlineStr"/>
+      <c r="EG4" t="inlineStr"/>
+      <c r="EH4" t="inlineStr"/>
+      <c r="EI4" t="inlineStr"/>
+      <c r="EJ4" t="inlineStr"/>
+      <c r="EK4" t="inlineStr"/>
+      <c r="EL4" t="inlineStr"/>
+      <c r="EM4" t="inlineStr"/>
+      <c r="EN4" t="inlineStr"/>
+      <c r="EO4" t="inlineStr"/>
+      <c r="EP4" t="inlineStr"/>
+      <c r="EQ4" t="inlineStr"/>
+      <c r="ER4" t="inlineStr"/>
+      <c r="ES4" t="inlineStr"/>
+      <c r="ET4" t="inlineStr"/>
+      <c r="EU4" t="inlineStr"/>
+      <c r="EV4" t="inlineStr"/>
+      <c r="EW4" t="inlineStr"/>
+      <c r="EX4" t="inlineStr"/>
+      <c r="EY4" t="inlineStr"/>
+      <c r="EZ4" t="inlineStr"/>
+      <c r="FA4" t="inlineStr"/>
+      <c r="FB4" t="inlineStr"/>
+      <c r="FC4" t="inlineStr"/>
+      <c r="FD4" t="inlineStr"/>
+      <c r="FE4" t="inlineStr"/>
+      <c r="FF4" t="inlineStr"/>
+      <c r="FG4" t="inlineStr"/>
+      <c r="FH4" t="inlineStr"/>
+      <c r="FI4" t="inlineStr"/>
+      <c r="FJ4" t="inlineStr"/>
+      <c r="FK4" t="inlineStr"/>
+      <c r="FL4" t="inlineStr"/>
+      <c r="FM4" t="inlineStr"/>
+      <c r="FN4" t="inlineStr"/>
+      <c r="FO4" t="inlineStr"/>
+      <c r="FP4" t="inlineStr"/>
+      <c r="FQ4" t="inlineStr"/>
+      <c r="FR4" t="inlineStr"/>
+      <c r="FS4" t="inlineStr"/>
+      <c r="FT4" t="inlineStr"/>
+      <c r="FU4" t="inlineStr"/>
+      <c r="FV4" t="inlineStr"/>
+      <c r="FW4" t="inlineStr"/>
+      <c r="FX4" t="inlineStr"/>
+      <c r="FY4" t="inlineStr"/>
+      <c r="FZ4" t="inlineStr"/>
+      <c r="GA4" t="inlineStr"/>
+      <c r="GB4" t="inlineStr"/>
+      <c r="GC4" t="inlineStr"/>
+      <c r="GD4" t="inlineStr"/>
+      <c r="GE4" t="inlineStr"/>
+      <c r="GF4" t="inlineStr"/>
+      <c r="GG4" t="inlineStr"/>
+      <c r="GH4" t="inlineStr"/>
+      <c r="GI4" t="inlineStr"/>
+      <c r="GJ4" t="inlineStr"/>
+      <c r="GK4" t="inlineStr"/>
+      <c r="GL4" t="inlineStr"/>
+      <c r="GM4" t="inlineStr"/>
+      <c r="GN4" t="inlineStr"/>
+      <c r="GO4" t="inlineStr"/>
+      <c r="GP4" t="inlineStr"/>
+      <c r="GQ4" t="inlineStr"/>
+      <c r="GR4" t="inlineStr"/>
+      <c r="GS4" t="inlineStr"/>
+      <c r="GT4" t="inlineStr"/>
+      <c r="GU4" t="inlineStr"/>
+      <c r="GV4" t="inlineStr"/>
+      <c r="GW4" t="inlineStr"/>
+      <c r="GX4" t="inlineStr"/>
+      <c r="GY4" t="inlineStr"/>
+      <c r="GZ4" t="inlineStr"/>
+      <c r="HA4" t="inlineStr"/>
+      <c r="HB4" t="inlineStr"/>
+      <c r="HC4" t="inlineStr"/>
+      <c r="HD4" t="inlineStr"/>
+      <c r="HE4" t="inlineStr"/>
+      <c r="HF4" t="inlineStr"/>
+      <c r="HG4" t="inlineStr"/>
+      <c r="HH4" t="inlineStr"/>
+      <c r="HI4" t="inlineStr"/>
+      <c r="HJ4" t="inlineStr"/>
+      <c r="HK4" t="inlineStr"/>
+      <c r="HL4" t="inlineStr"/>
+      <c r="HM4" t="inlineStr"/>
+      <c r="HN4" t="inlineStr"/>
+      <c r="HO4" t="inlineStr"/>
+      <c r="HP4" t="inlineStr"/>
+      <c r="HQ4" t="inlineStr"/>
+      <c r="HR4" t="inlineStr"/>
+      <c r="HS4" t="inlineStr"/>
+      <c r="HT4" t="inlineStr"/>
+      <c r="HU4" t="inlineStr"/>
+      <c r="HV4" t="inlineStr"/>
+      <c r="HW4" t="inlineStr"/>
+      <c r="HX4" t="inlineStr"/>
+      <c r="HY4" t="inlineStr"/>
+      <c r="HZ4" t="inlineStr"/>
+      <c r="IA4" t="inlineStr"/>
+      <c r="IB4" t="inlineStr"/>
+      <c r="IC4" t="inlineStr"/>
+      <c r="ID4" t="inlineStr"/>
+      <c r="IE4" t="inlineStr"/>
+      <c r="IF4" t="inlineStr"/>
+      <c r="IG4" t="inlineStr"/>
+      <c r="IH4" t="inlineStr"/>
+      <c r="II4" t="inlineStr"/>
+      <c r="IJ4" t="inlineStr"/>
+      <c r="IK4" t="inlineStr"/>
+      <c r="IL4" t="inlineStr"/>
+      <c r="IM4" t="inlineStr"/>
+      <c r="IN4" t="inlineStr"/>
+      <c r="IO4" t="inlineStr"/>
+      <c r="IP4" t="inlineStr"/>
+      <c r="IQ4" t="inlineStr"/>
+      <c r="IR4" t="inlineStr"/>
+      <c r="IS4" t="inlineStr"/>
+      <c r="IT4" t="inlineStr"/>
+      <c r="IU4" t="inlineStr"/>
+      <c r="IV4" t="inlineStr"/>
+      <c r="IW4" t="inlineStr"/>
+      <c r="IX4" t="inlineStr"/>
+      <c r="IY4" t="inlineStr"/>
+      <c r="IZ4" t="inlineStr"/>
+      <c r="JA4" t="inlineStr"/>
+      <c r="JB4" t="inlineStr"/>
+      <c r="JC4" t="inlineStr"/>
+      <c r="JD4" t="inlineStr"/>
+      <c r="JE4" t="inlineStr"/>
+      <c r="JF4" t="inlineStr"/>
+      <c r="JG4" t="inlineStr"/>
+      <c r="JH4" t="inlineStr"/>
+      <c r="JI4" t="inlineStr"/>
+      <c r="JJ4" t="inlineStr"/>
+      <c r="JK4" t="inlineStr"/>
+      <c r="JL4" t="inlineStr"/>
+      <c r="JM4" t="inlineStr"/>
+      <c r="JN4" t="inlineStr"/>
+      <c r="JO4" t="inlineStr"/>
+      <c r="JP4" t="inlineStr"/>
+      <c r="JQ4" t="inlineStr"/>
+      <c r="JR4" t="inlineStr"/>
+      <c r="JS4" t="inlineStr"/>
+      <c r="JT4" t="inlineStr"/>
+      <c r="JU4" t="inlineStr"/>
+      <c r="JV4" t="inlineStr"/>
+      <c r="JW4" t="inlineStr"/>
+      <c r="JX4" t="inlineStr"/>
+      <c r="JY4" t="inlineStr"/>
+      <c r="JZ4" t="inlineStr"/>
+      <c r="KA4" t="inlineStr"/>
+      <c r="KB4" t="inlineStr"/>
+      <c r="KC4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
@@ -2580,7 +2745,7 @@
         <v>3791.442857142857</v>
       </c>
       <c r="BA5" t="n">
-        <v>3674.528571428572</v>
+        <v>3674.528571428571</v>
       </c>
       <c r="BB5" t="n">
         <v>3559.957142857143</v>
@@ -2604,7 +2769,7 @@
         <v>2921.971428571429</v>
       </c>
       <c r="BI5" t="n">
-        <v>2824.228571428572</v>
+        <v>2824.228571428571</v>
       </c>
       <c r="BJ5" t="n">
         <v>2731.842857142857</v>
@@ -2616,7 +2781,7 @@
         <v>2539.3</v>
       </c>
       <c r="BM5" t="n">
-        <v>2444.157142857144</v>
+        <v>2444.157142857143</v>
       </c>
       <c r="BN5" t="n">
         <v>2350.6</v>
@@ -3045,7 +3210,7 @@
         <v>378.5857142857143</v>
       </c>
       <c r="GZ5" t="n">
-        <v>408.3428571428572</v>
+        <v>408.3428571428571</v>
       </c>
       <c r="HA5" t="n">
         <v>440.4714285714286</v>
@@ -3135,7 +3300,7 @@
         <v>2248.842857142857</v>
       </c>
       <c r="ID5" t="n">
-        <v>2342.514285714285</v>
+        <v>2342.514285714286</v>
       </c>
       <c r="IE5" t="n">
         <v>2438.085714285714</v>
@@ -3150,7 +3315,7 @@
         <v>2748.328571428571</v>
       </c>
       <c r="II5" t="n">
-        <v>2853.014285714285</v>
+        <v>2853.014285714286</v>
       </c>
       <c r="IJ5" t="n">
         <v>2956.157142857143</v>
@@ -3219,7 +3384,7 @@
         <v>5165.2</v>
       </c>
       <c r="JF5" t="n">
-        <v>5269.957142857144</v>
+        <v>5269.957142857143</v>
       </c>
       <c r="JG5" t="n">
         <v>5371.385714285714</v>
@@ -3832,10 +3997,10 @@
         <v>52.62857142857143</v>
       </c>
       <c r="FX6" t="n">
-        <v>53.02857142857143</v>
+        <v>53.02857142857142</v>
       </c>
       <c r="FY6" t="n">
-        <v>48.22857142857144</v>
+        <v>48.22857142857143</v>
       </c>
       <c r="FZ6" t="n">
         <v>46.67142857142857</v>
@@ -3856,7 +4021,7 @@
         <v>48.55714285714286</v>
       </c>
       <c r="GF6" t="n">
-        <v>40.22857142857144</v>
+        <v>40.22857142857143</v>
       </c>
       <c r="GG6" t="n">
         <v>36.05714285714286</v>
@@ -3907,7 +4072,7 @@
         <v>15.07142857142857</v>
       </c>
       <c r="GW6" t="n">
-        <v>18.81428571428572</v>
+        <v>18.81428571428571</v>
       </c>
       <c r="GX6" t="n">
         <v>13.52857142857143</v>
@@ -4024,7 +4189,7 @@
         <v>3.671428571428571</v>
       </c>
       <c r="IJ6" t="n">
-        <v>4.9</v>
+        <v>4.899999999999999</v>
       </c>
       <c r="IK6" t="n">
         <v>2.328571428571429</v>
@@ -4370,7 +4535,7 @@
         <v>11.9</v>
       </c>
       <c r="BQ7" t="n">
-        <v>23.81428571428572</v>
+        <v>23.81428571428571</v>
       </c>
       <c r="BR7" t="n">
         <v>35.71428571428572</v>
@@ -4385,7 +4550,7 @@
         <v>35.71428571428572</v>
       </c>
       <c r="BV7" t="n">
-        <v>23.81428571428572</v>
+        <v>23.81428571428571</v>
       </c>
       <c r="BW7" t="n">
         <v>11.9</v>
@@ -4466,7 +4631,7 @@
         <v>11.9</v>
       </c>
       <c r="CW7" t="n">
-        <v>23.81428571428572</v>
+        <v>23.81428571428571</v>
       </c>
       <c r="CX7" t="n">
         <v>35.71428571428572</v>
@@ -4478,10 +4643,10 @@
         <v>52.34285714285715</v>
       </c>
       <c r="DA7" t="n">
-        <v>59.52857142857143</v>
+        <v>59.52857142857142</v>
       </c>
       <c r="DB7" t="n">
-        <v>59.52857142857143</v>
+        <v>59.52857142857142</v>
       </c>
       <c r="DC7" t="n">
         <v>50.1</v>
@@ -4493,7 +4658,7 @@
         <v>35.71428571428572</v>
       </c>
       <c r="DF7" t="n">
-        <v>23.81428571428572</v>
+        <v>23.81428571428571</v>
       </c>
       <c r="DG7" t="n">
         <v>23.8</v>
@@ -4679,7 +4844,7 @@
         <v>522.3142857142857</v>
       </c>
       <c r="FP7" t="n">
-        <v>419.3428571428572</v>
+        <v>419.3428571428571</v>
       </c>
       <c r="FQ7" t="n">
         <v>312.1857142857143</v>
@@ -4952,7 +5117,7 @@
         <v>460.7571428571429</v>
       </c>
       <c r="JC7" t="n">
-        <v>438.3428571428572</v>
+        <v>438.3428571428571</v>
       </c>
       <c r="JD7" t="n">
         <v>409.4142857142857</v>
@@ -4985,7 +5150,7 @@
         <v>130.9571428571429</v>
       </c>
       <c r="JN7" t="n">
-        <v>190.0428571428572</v>
+        <v>190.0428571428571</v>
       </c>
       <c r="JO7" t="n">
         <v>249.5571428571429</v>
@@ -5000,7 +5165,7 @@
         <v>309.0142857142857</v>
       </c>
       <c r="JS7" t="n">
-        <v>248.5428571428572</v>
+        <v>248.5428571428571</v>
       </c>
       <c r="JT7" t="n">
         <v>201.0857142857142</v>
@@ -5030,11 +5195,299 @@
         <v>202.3857142857143</v>
       </c>
       <c r="KC7" t="n">
-        <v>235.6428571428572</v>
+        <v>235.6428571428571</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
+      <c r="X8" t="inlineStr"/>
+      <c r="Y8" t="inlineStr"/>
+      <c r="Z8" t="inlineStr"/>
+      <c r="AA8" t="inlineStr"/>
+      <c r="AB8" t="inlineStr"/>
+      <c r="AC8" t="inlineStr"/>
+      <c r="AD8" t="inlineStr"/>
+      <c r="AE8" t="inlineStr"/>
+      <c r="AF8" t="inlineStr"/>
+      <c r="AG8" t="inlineStr"/>
+      <c r="AH8" t="inlineStr"/>
+      <c r="AI8" t="inlineStr"/>
+      <c r="AJ8" t="inlineStr"/>
+      <c r="AK8" t="inlineStr"/>
+      <c r="AL8" t="inlineStr"/>
+      <c r="AM8" t="inlineStr"/>
+      <c r="AN8" t="inlineStr"/>
+      <c r="AO8" t="inlineStr"/>
+      <c r="AP8" t="inlineStr"/>
+      <c r="AQ8" t="inlineStr"/>
+      <c r="AR8" t="inlineStr"/>
+      <c r="AS8" t="inlineStr"/>
+      <c r="AT8" t="inlineStr"/>
+      <c r="AU8" t="inlineStr"/>
+      <c r="AV8" t="inlineStr"/>
+      <c r="AW8" t="inlineStr"/>
+      <c r="AX8" t="inlineStr"/>
+      <c r="AY8" t="inlineStr"/>
+      <c r="AZ8" t="inlineStr"/>
+      <c r="BA8" t="inlineStr"/>
+      <c r="BB8" t="inlineStr"/>
+      <c r="BC8" t="inlineStr"/>
+      <c r="BD8" t="inlineStr"/>
+      <c r="BE8" t="inlineStr"/>
+      <c r="BF8" t="inlineStr"/>
+      <c r="BG8" t="inlineStr"/>
+      <c r="BH8" t="inlineStr"/>
+      <c r="BI8" t="inlineStr"/>
+      <c r="BJ8" t="inlineStr"/>
+      <c r="BK8" t="inlineStr"/>
+      <c r="BL8" t="inlineStr"/>
+      <c r="BM8" t="inlineStr"/>
+      <c r="BN8" t="inlineStr"/>
+      <c r="BO8" t="inlineStr"/>
+      <c r="BP8" t="inlineStr"/>
+      <c r="BQ8" t="inlineStr"/>
+      <c r="BR8" t="inlineStr"/>
+      <c r="BS8" t="inlineStr"/>
+      <c r="BT8" t="inlineStr"/>
+      <c r="BU8" t="inlineStr"/>
+      <c r="BV8" t="inlineStr"/>
+      <c r="BW8" t="inlineStr"/>
+      <c r="BX8" t="inlineStr"/>
+      <c r="BY8" t="inlineStr"/>
+      <c r="BZ8" t="inlineStr"/>
+      <c r="CA8" t="inlineStr"/>
+      <c r="CB8" t="inlineStr"/>
+      <c r="CC8" t="inlineStr"/>
+      <c r="CD8" t="inlineStr"/>
+      <c r="CE8" t="inlineStr"/>
+      <c r="CF8" t="inlineStr"/>
+      <c r="CG8" t="inlineStr"/>
+      <c r="CH8" t="inlineStr"/>
+      <c r="CI8" t="inlineStr"/>
+      <c r="CJ8" t="inlineStr"/>
+      <c r="CK8" t="inlineStr"/>
+      <c r="CL8" t="inlineStr"/>
+      <c r="CM8" t="inlineStr"/>
+      <c r="CN8" t="inlineStr"/>
+      <c r="CO8" t="inlineStr"/>
+      <c r="CP8" t="inlineStr"/>
+      <c r="CQ8" t="inlineStr"/>
+      <c r="CR8" t="inlineStr"/>
+      <c r="CS8" t="inlineStr"/>
+      <c r="CT8" t="inlineStr"/>
+      <c r="CU8" t="inlineStr"/>
+      <c r="CV8" t="inlineStr"/>
+      <c r="CW8" t="inlineStr"/>
+      <c r="CX8" t="inlineStr"/>
+      <c r="CY8" t="inlineStr"/>
+      <c r="CZ8" t="inlineStr"/>
+      <c r="DA8" t="inlineStr"/>
+      <c r="DB8" t="inlineStr"/>
+      <c r="DC8" t="inlineStr"/>
+      <c r="DD8" t="inlineStr"/>
+      <c r="DE8" t="inlineStr"/>
+      <c r="DF8" t="inlineStr"/>
+      <c r="DG8" t="inlineStr"/>
+      <c r="DH8" t="inlineStr"/>
+      <c r="DI8" t="inlineStr"/>
+      <c r="DJ8" t="inlineStr"/>
+      <c r="DK8" t="inlineStr"/>
+      <c r="DL8" t="inlineStr"/>
+      <c r="DM8" t="inlineStr"/>
+      <c r="DN8" t="inlineStr"/>
+      <c r="DO8" t="inlineStr"/>
+      <c r="DP8" t="inlineStr"/>
+      <c r="DQ8" t="inlineStr"/>
+      <c r="DR8" t="inlineStr"/>
+      <c r="DS8" t="inlineStr"/>
+      <c r="DT8" t="inlineStr"/>
+      <c r="DU8" t="inlineStr"/>
+      <c r="DV8" t="inlineStr"/>
+      <c r="DW8" t="inlineStr"/>
+      <c r="DX8" t="inlineStr"/>
+      <c r="DY8" t="inlineStr"/>
+      <c r="DZ8" t="inlineStr"/>
+      <c r="EA8" t="inlineStr"/>
+      <c r="EB8" t="inlineStr"/>
+      <c r="EC8" t="inlineStr"/>
+      <c r="ED8" t="inlineStr"/>
+      <c r="EE8" t="inlineStr"/>
+      <c r="EF8" t="inlineStr"/>
+      <c r="EG8" t="inlineStr"/>
+      <c r="EH8" t="inlineStr"/>
+      <c r="EI8" t="inlineStr"/>
+      <c r="EJ8" t="inlineStr"/>
+      <c r="EK8" t="inlineStr"/>
+      <c r="EL8" t="inlineStr"/>
+      <c r="EM8" t="inlineStr"/>
+      <c r="EN8" t="inlineStr"/>
+      <c r="EO8" t="inlineStr"/>
+      <c r="EP8" t="inlineStr"/>
+      <c r="EQ8" t="inlineStr"/>
+      <c r="ER8" t="inlineStr"/>
+      <c r="ES8" t="inlineStr"/>
+      <c r="ET8" t="inlineStr"/>
+      <c r="EU8" t="inlineStr"/>
+      <c r="EV8" t="inlineStr"/>
+      <c r="EW8" t="inlineStr"/>
+      <c r="EX8" t="inlineStr"/>
+      <c r="EY8" t="inlineStr"/>
+      <c r="EZ8" t="inlineStr"/>
+      <c r="FA8" t="inlineStr"/>
+      <c r="FB8" t="inlineStr"/>
+      <c r="FC8" t="inlineStr"/>
+      <c r="FD8" t="inlineStr"/>
+      <c r="FE8" t="inlineStr"/>
+      <c r="FF8" t="inlineStr"/>
+      <c r="FG8" t="inlineStr"/>
+      <c r="FH8" t="inlineStr"/>
+      <c r="FI8" t="inlineStr"/>
+      <c r="FJ8" t="inlineStr"/>
+      <c r="FK8" t="inlineStr"/>
+      <c r="FL8" t="inlineStr"/>
+      <c r="FM8" t="inlineStr"/>
+      <c r="FN8" t="inlineStr"/>
+      <c r="FO8" t="inlineStr"/>
+      <c r="FP8" t="inlineStr"/>
+      <c r="FQ8" t="inlineStr"/>
+      <c r="FR8" t="inlineStr"/>
+      <c r="FS8" t="inlineStr"/>
+      <c r="FT8" t="inlineStr"/>
+      <c r="FU8" t="inlineStr"/>
+      <c r="FV8" t="inlineStr"/>
+      <c r="FW8" t="inlineStr"/>
+      <c r="FX8" t="inlineStr"/>
+      <c r="FY8" t="inlineStr"/>
+      <c r="FZ8" t="inlineStr"/>
+      <c r="GA8" t="inlineStr"/>
+      <c r="GB8" t="inlineStr"/>
+      <c r="GC8" t="inlineStr"/>
+      <c r="GD8" t="inlineStr"/>
+      <c r="GE8" t="inlineStr"/>
+      <c r="GF8" t="inlineStr"/>
+      <c r="GG8" t="inlineStr"/>
+      <c r="GH8" t="inlineStr"/>
+      <c r="GI8" t="inlineStr"/>
+      <c r="GJ8" t="inlineStr"/>
+      <c r="GK8" t="inlineStr"/>
+      <c r="GL8" t="inlineStr"/>
+      <c r="GM8" t="inlineStr"/>
+      <c r="GN8" t="inlineStr"/>
+      <c r="GO8" t="inlineStr"/>
+      <c r="GP8" t="inlineStr"/>
+      <c r="GQ8" t="inlineStr"/>
+      <c r="GR8" t="inlineStr"/>
+      <c r="GS8" t="inlineStr"/>
+      <c r="GT8" t="inlineStr"/>
+      <c r="GU8" t="inlineStr"/>
+      <c r="GV8" t="inlineStr"/>
+      <c r="GW8" t="inlineStr"/>
+      <c r="GX8" t="inlineStr"/>
+      <c r="GY8" t="inlineStr"/>
+      <c r="GZ8" t="inlineStr"/>
+      <c r="HA8" t="inlineStr"/>
+      <c r="HB8" t="inlineStr"/>
+      <c r="HC8" t="inlineStr"/>
+      <c r="HD8" t="inlineStr"/>
+      <c r="HE8" t="inlineStr"/>
+      <c r="HF8" t="inlineStr"/>
+      <c r="HG8" t="inlineStr"/>
+      <c r="HH8" t="inlineStr"/>
+      <c r="HI8" t="inlineStr"/>
+      <c r="HJ8" t="inlineStr"/>
+      <c r="HK8" t="inlineStr"/>
+      <c r="HL8" t="inlineStr"/>
+      <c r="HM8" t="inlineStr"/>
+      <c r="HN8" t="inlineStr"/>
+      <c r="HO8" t="inlineStr"/>
+      <c r="HP8" t="inlineStr"/>
+      <c r="HQ8" t="inlineStr"/>
+      <c r="HR8" t="inlineStr"/>
+      <c r="HS8" t="inlineStr"/>
+      <c r="HT8" t="inlineStr"/>
+      <c r="HU8" t="inlineStr"/>
+      <c r="HV8" t="inlineStr"/>
+      <c r="HW8" t="inlineStr"/>
+      <c r="HX8" t="inlineStr"/>
+      <c r="HY8" t="inlineStr"/>
+      <c r="HZ8" t="inlineStr"/>
+      <c r="IA8" t="inlineStr"/>
+      <c r="IB8" t="inlineStr"/>
+      <c r="IC8" t="inlineStr"/>
+      <c r="ID8" t="inlineStr"/>
+      <c r="IE8" t="inlineStr"/>
+      <c r="IF8" t="inlineStr"/>
+      <c r="IG8" t="inlineStr"/>
+      <c r="IH8" t="inlineStr"/>
+      <c r="II8" t="inlineStr"/>
+      <c r="IJ8" t="inlineStr"/>
+      <c r="IK8" t="inlineStr"/>
+      <c r="IL8" t="inlineStr"/>
+      <c r="IM8" t="inlineStr"/>
+      <c r="IN8" t="inlineStr"/>
+      <c r="IO8" t="inlineStr"/>
+      <c r="IP8" t="inlineStr"/>
+      <c r="IQ8" t="inlineStr"/>
+      <c r="IR8" t="inlineStr"/>
+      <c r="IS8" t="inlineStr"/>
+      <c r="IT8" t="inlineStr"/>
+      <c r="IU8" t="inlineStr"/>
+      <c r="IV8" t="inlineStr"/>
+      <c r="IW8" t="inlineStr"/>
+      <c r="IX8" t="inlineStr"/>
+      <c r="IY8" t="inlineStr"/>
+      <c r="IZ8" t="inlineStr"/>
+      <c r="JA8" t="inlineStr"/>
+      <c r="JB8" t="inlineStr"/>
+      <c r="JC8" t="inlineStr"/>
+      <c r="JD8" t="inlineStr"/>
+      <c r="JE8" t="inlineStr"/>
+      <c r="JF8" t="inlineStr"/>
+      <c r="JG8" t="inlineStr"/>
+      <c r="JH8" t="inlineStr"/>
+      <c r="JI8" t="inlineStr"/>
+      <c r="JJ8" t="inlineStr"/>
+      <c r="JK8" t="inlineStr"/>
+      <c r="JL8" t="inlineStr"/>
+      <c r="JM8" t="inlineStr"/>
+      <c r="JN8" t="inlineStr"/>
+      <c r="JO8" t="inlineStr"/>
+      <c r="JP8" t="inlineStr"/>
+      <c r="JQ8" t="inlineStr"/>
+      <c r="JR8" t="inlineStr"/>
+      <c r="JS8" t="inlineStr"/>
+      <c r="JT8" t="inlineStr"/>
+      <c r="JU8" t="inlineStr"/>
+      <c r="JV8" t="inlineStr"/>
+      <c r="JW8" t="inlineStr"/>
+      <c r="JX8" t="inlineStr"/>
+      <c r="JY8" t="inlineStr"/>
+      <c r="JZ8" t="inlineStr"/>
+      <c r="KA8" t="inlineStr"/>
+      <c r="KB8" t="inlineStr"/>
+      <c r="KC8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
@@ -5909,6 +6362,294 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr"/>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
+      <c r="X10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr"/>
+      <c r="Z10" t="inlineStr"/>
+      <c r="AA10" t="inlineStr"/>
+      <c r="AB10" t="inlineStr"/>
+      <c r="AC10" t="inlineStr"/>
+      <c r="AD10" t="inlineStr"/>
+      <c r="AE10" t="inlineStr"/>
+      <c r="AF10" t="inlineStr"/>
+      <c r="AG10" t="inlineStr"/>
+      <c r="AH10" t="inlineStr"/>
+      <c r="AI10" t="inlineStr"/>
+      <c r="AJ10" t="inlineStr"/>
+      <c r="AK10" t="inlineStr"/>
+      <c r="AL10" t="inlineStr"/>
+      <c r="AM10" t="inlineStr"/>
+      <c r="AN10" t="inlineStr"/>
+      <c r="AO10" t="inlineStr"/>
+      <c r="AP10" t="inlineStr"/>
+      <c r="AQ10" t="inlineStr"/>
+      <c r="AR10" t="inlineStr"/>
+      <c r="AS10" t="inlineStr"/>
+      <c r="AT10" t="inlineStr"/>
+      <c r="AU10" t="inlineStr"/>
+      <c r="AV10" t="inlineStr"/>
+      <c r="AW10" t="inlineStr"/>
+      <c r="AX10" t="inlineStr"/>
+      <c r="AY10" t="inlineStr"/>
+      <c r="AZ10" t="inlineStr"/>
+      <c r="BA10" t="inlineStr"/>
+      <c r="BB10" t="inlineStr"/>
+      <c r="BC10" t="inlineStr"/>
+      <c r="BD10" t="inlineStr"/>
+      <c r="BE10" t="inlineStr"/>
+      <c r="BF10" t="inlineStr"/>
+      <c r="BG10" t="inlineStr"/>
+      <c r="BH10" t="inlineStr"/>
+      <c r="BI10" t="inlineStr"/>
+      <c r="BJ10" t="inlineStr"/>
+      <c r="BK10" t="inlineStr"/>
+      <c r="BL10" t="inlineStr"/>
+      <c r="BM10" t="inlineStr"/>
+      <c r="BN10" t="inlineStr"/>
+      <c r="BO10" t="inlineStr"/>
+      <c r="BP10" t="inlineStr"/>
+      <c r="BQ10" t="inlineStr"/>
+      <c r="BR10" t="inlineStr"/>
+      <c r="BS10" t="inlineStr"/>
+      <c r="BT10" t="inlineStr"/>
+      <c r="BU10" t="inlineStr"/>
+      <c r="BV10" t="inlineStr"/>
+      <c r="BW10" t="inlineStr"/>
+      <c r="BX10" t="inlineStr"/>
+      <c r="BY10" t="inlineStr"/>
+      <c r="BZ10" t="inlineStr"/>
+      <c r="CA10" t="inlineStr"/>
+      <c r="CB10" t="inlineStr"/>
+      <c r="CC10" t="inlineStr"/>
+      <c r="CD10" t="inlineStr"/>
+      <c r="CE10" t="inlineStr"/>
+      <c r="CF10" t="inlineStr"/>
+      <c r="CG10" t="inlineStr"/>
+      <c r="CH10" t="inlineStr"/>
+      <c r="CI10" t="inlineStr"/>
+      <c r="CJ10" t="inlineStr"/>
+      <c r="CK10" t="inlineStr"/>
+      <c r="CL10" t="inlineStr"/>
+      <c r="CM10" t="inlineStr"/>
+      <c r="CN10" t="inlineStr"/>
+      <c r="CO10" t="inlineStr"/>
+      <c r="CP10" t="inlineStr"/>
+      <c r="CQ10" t="inlineStr"/>
+      <c r="CR10" t="inlineStr"/>
+      <c r="CS10" t="inlineStr"/>
+      <c r="CT10" t="inlineStr"/>
+      <c r="CU10" t="inlineStr"/>
+      <c r="CV10" t="inlineStr"/>
+      <c r="CW10" t="inlineStr"/>
+      <c r="CX10" t="inlineStr"/>
+      <c r="CY10" t="inlineStr"/>
+      <c r="CZ10" t="inlineStr"/>
+      <c r="DA10" t="inlineStr"/>
+      <c r="DB10" t="inlineStr"/>
+      <c r="DC10" t="inlineStr"/>
+      <c r="DD10" t="inlineStr"/>
+      <c r="DE10" t="inlineStr"/>
+      <c r="DF10" t="inlineStr"/>
+      <c r="DG10" t="inlineStr"/>
+      <c r="DH10" t="inlineStr"/>
+      <c r="DI10" t="inlineStr"/>
+      <c r="DJ10" t="inlineStr"/>
+      <c r="DK10" t="inlineStr"/>
+      <c r="DL10" t="inlineStr"/>
+      <c r="DM10" t="inlineStr"/>
+      <c r="DN10" t="inlineStr"/>
+      <c r="DO10" t="inlineStr"/>
+      <c r="DP10" t="inlineStr"/>
+      <c r="DQ10" t="inlineStr"/>
+      <c r="DR10" t="inlineStr"/>
+      <c r="DS10" t="inlineStr"/>
+      <c r="DT10" t="inlineStr"/>
+      <c r="DU10" t="inlineStr"/>
+      <c r="DV10" t="inlineStr"/>
+      <c r="DW10" t="inlineStr"/>
+      <c r="DX10" t="inlineStr"/>
+      <c r="DY10" t="inlineStr"/>
+      <c r="DZ10" t="inlineStr"/>
+      <c r="EA10" t="inlineStr"/>
+      <c r="EB10" t="inlineStr"/>
+      <c r="EC10" t="inlineStr"/>
+      <c r="ED10" t="inlineStr"/>
+      <c r="EE10" t="inlineStr"/>
+      <c r="EF10" t="inlineStr"/>
+      <c r="EG10" t="inlineStr"/>
+      <c r="EH10" t="inlineStr"/>
+      <c r="EI10" t="inlineStr"/>
+      <c r="EJ10" t="inlineStr"/>
+      <c r="EK10" t="inlineStr"/>
+      <c r="EL10" t="inlineStr"/>
+      <c r="EM10" t="inlineStr"/>
+      <c r="EN10" t="inlineStr"/>
+      <c r="EO10" t="inlineStr"/>
+      <c r="EP10" t="inlineStr"/>
+      <c r="EQ10" t="inlineStr"/>
+      <c r="ER10" t="inlineStr"/>
+      <c r="ES10" t="inlineStr"/>
+      <c r="ET10" t="inlineStr"/>
+      <c r="EU10" t="inlineStr"/>
+      <c r="EV10" t="inlineStr"/>
+      <c r="EW10" t="inlineStr"/>
+      <c r="EX10" t="inlineStr"/>
+      <c r="EY10" t="inlineStr"/>
+      <c r="EZ10" t="inlineStr"/>
+      <c r="FA10" t="inlineStr"/>
+      <c r="FB10" t="inlineStr"/>
+      <c r="FC10" t="inlineStr"/>
+      <c r="FD10" t="inlineStr"/>
+      <c r="FE10" t="inlineStr"/>
+      <c r="FF10" t="inlineStr"/>
+      <c r="FG10" t="inlineStr"/>
+      <c r="FH10" t="inlineStr"/>
+      <c r="FI10" t="inlineStr"/>
+      <c r="FJ10" t="inlineStr"/>
+      <c r="FK10" t="inlineStr"/>
+      <c r="FL10" t="inlineStr"/>
+      <c r="FM10" t="inlineStr"/>
+      <c r="FN10" t="inlineStr"/>
+      <c r="FO10" t="inlineStr"/>
+      <c r="FP10" t="inlineStr"/>
+      <c r="FQ10" t="inlineStr"/>
+      <c r="FR10" t="inlineStr"/>
+      <c r="FS10" t="inlineStr"/>
+      <c r="FT10" t="inlineStr"/>
+      <c r="FU10" t="inlineStr"/>
+      <c r="FV10" t="inlineStr"/>
+      <c r="FW10" t="inlineStr"/>
+      <c r="FX10" t="inlineStr"/>
+      <c r="FY10" t="inlineStr"/>
+      <c r="FZ10" t="inlineStr"/>
+      <c r="GA10" t="inlineStr"/>
+      <c r="GB10" t="inlineStr"/>
+      <c r="GC10" t="inlineStr"/>
+      <c r="GD10" t="inlineStr"/>
+      <c r="GE10" t="inlineStr"/>
+      <c r="GF10" t="inlineStr"/>
+      <c r="GG10" t="inlineStr"/>
+      <c r="GH10" t="inlineStr"/>
+      <c r="GI10" t="inlineStr"/>
+      <c r="GJ10" t="inlineStr"/>
+      <c r="GK10" t="inlineStr"/>
+      <c r="GL10" t="inlineStr"/>
+      <c r="GM10" t="inlineStr"/>
+      <c r="GN10" t="inlineStr"/>
+      <c r="GO10" t="inlineStr"/>
+      <c r="GP10" t="inlineStr"/>
+      <c r="GQ10" t="inlineStr"/>
+      <c r="GR10" t="inlineStr"/>
+      <c r="GS10" t="inlineStr"/>
+      <c r="GT10" t="inlineStr"/>
+      <c r="GU10" t="inlineStr"/>
+      <c r="GV10" t="inlineStr"/>
+      <c r="GW10" t="inlineStr"/>
+      <c r="GX10" t="inlineStr"/>
+      <c r="GY10" t="inlineStr"/>
+      <c r="GZ10" t="inlineStr"/>
+      <c r="HA10" t="inlineStr"/>
+      <c r="HB10" t="inlineStr"/>
+      <c r="HC10" t="inlineStr"/>
+      <c r="HD10" t="inlineStr"/>
+      <c r="HE10" t="inlineStr"/>
+      <c r="HF10" t="inlineStr"/>
+      <c r="HG10" t="inlineStr"/>
+      <c r="HH10" t="inlineStr"/>
+      <c r="HI10" t="inlineStr"/>
+      <c r="HJ10" t="inlineStr"/>
+      <c r="HK10" t="inlineStr"/>
+      <c r="HL10" t="inlineStr"/>
+      <c r="HM10" t="inlineStr"/>
+      <c r="HN10" t="inlineStr"/>
+      <c r="HO10" t="inlineStr"/>
+      <c r="HP10" t="inlineStr"/>
+      <c r="HQ10" t="inlineStr"/>
+      <c r="HR10" t="inlineStr"/>
+      <c r="HS10" t="inlineStr"/>
+      <c r="HT10" t="inlineStr"/>
+      <c r="HU10" t="inlineStr"/>
+      <c r="HV10" t="inlineStr"/>
+      <c r="HW10" t="inlineStr"/>
+      <c r="HX10" t="inlineStr"/>
+      <c r="HY10" t="inlineStr"/>
+      <c r="HZ10" t="inlineStr"/>
+      <c r="IA10" t="inlineStr"/>
+      <c r="IB10" t="inlineStr"/>
+      <c r="IC10" t="inlineStr"/>
+      <c r="ID10" t="inlineStr"/>
+      <c r="IE10" t="inlineStr"/>
+      <c r="IF10" t="inlineStr"/>
+      <c r="IG10" t="inlineStr"/>
+      <c r="IH10" t="inlineStr"/>
+      <c r="II10" t="inlineStr"/>
+      <c r="IJ10" t="inlineStr"/>
+      <c r="IK10" t="inlineStr"/>
+      <c r="IL10" t="inlineStr"/>
+      <c r="IM10" t="inlineStr"/>
+      <c r="IN10" t="inlineStr"/>
+      <c r="IO10" t="inlineStr"/>
+      <c r="IP10" t="inlineStr"/>
+      <c r="IQ10" t="inlineStr"/>
+      <c r="IR10" t="inlineStr"/>
+      <c r="IS10" t="inlineStr"/>
+      <c r="IT10" t="inlineStr"/>
+      <c r="IU10" t="inlineStr"/>
+      <c r="IV10" t="inlineStr"/>
+      <c r="IW10" t="inlineStr"/>
+      <c r="IX10" t="inlineStr"/>
+      <c r="IY10" t="inlineStr"/>
+      <c r="IZ10" t="inlineStr"/>
+      <c r="JA10" t="inlineStr"/>
+      <c r="JB10" t="inlineStr"/>
+      <c r="JC10" t="inlineStr"/>
+      <c r="JD10" t="inlineStr"/>
+      <c r="JE10" t="inlineStr"/>
+      <c r="JF10" t="inlineStr"/>
+      <c r="JG10" t="inlineStr"/>
+      <c r="JH10" t="inlineStr"/>
+      <c r="JI10" t="inlineStr"/>
+      <c r="JJ10" t="inlineStr"/>
+      <c r="JK10" t="inlineStr"/>
+      <c r="JL10" t="inlineStr"/>
+      <c r="JM10" t="inlineStr"/>
+      <c r="JN10" t="inlineStr"/>
+      <c r="JO10" t="inlineStr"/>
+      <c r="JP10" t="inlineStr"/>
+      <c r="JQ10" t="inlineStr"/>
+      <c r="JR10" t="inlineStr"/>
+      <c r="JS10" t="inlineStr"/>
+      <c r="JT10" t="inlineStr"/>
+      <c r="JU10" t="inlineStr"/>
+      <c r="JV10" t="inlineStr"/>
+      <c r="JW10" t="inlineStr"/>
+      <c r="JX10" t="inlineStr"/>
+      <c r="JY10" t="inlineStr"/>
+      <c r="JZ10" t="inlineStr"/>
+      <c r="KA10" t="inlineStr"/>
+      <c r="KB10" t="inlineStr"/>
+      <c r="KC10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -6070,7 +6811,7 @@
         <v>3791.442857142857</v>
       </c>
       <c r="BA11" t="n">
-        <v>3674.528571428572</v>
+        <v>3674.528571428571</v>
       </c>
       <c r="BB11" t="n">
         <v>3559.957142857143</v>
@@ -6094,7 +6835,7 @@
         <v>2921.971428571429</v>
       </c>
       <c r="BI11" t="n">
-        <v>2824.228571428572</v>
+        <v>2824.228571428571</v>
       </c>
       <c r="BJ11" t="n">
         <v>2731.842857142857</v>
@@ -6106,7 +6847,7 @@
         <v>2539.3</v>
       </c>
       <c r="BM11" t="n">
-        <v>2444.157142857144</v>
+        <v>2444.157142857143</v>
       </c>
       <c r="BN11" t="n">
         <v>2350.6</v>
@@ -6127,7 +6868,7 @@
         <v>1916.014285714286</v>
       </c>
       <c r="BT11" t="n">
-        <v>1830.314285714285</v>
+        <v>1830.314285714286</v>
       </c>
       <c r="BU11" t="n">
         <v>1734.014285714286</v>
@@ -6289,7 +7030,7 @@
         <v>418.4142857142857</v>
       </c>
       <c r="DV11" t="n">
-        <v>425.8428571428572</v>
+        <v>425.8428571428571</v>
       </c>
       <c r="DW11" t="n">
         <v>465</v>
@@ -6595,7 +7336,7 @@
         <v>1825.071428571429</v>
       </c>
       <c r="HT11" t="n">
-        <v>1850.428571428572</v>
+        <v>1850.428571428571</v>
       </c>
       <c r="HU11" t="n">
         <v>1961.142857142857</v>
@@ -6706,7 +7447,7 @@
         <v>5465.099999999999</v>
       </c>
       <c r="JE11" t="n">
-        <v>5552.957142857144</v>
+        <v>5552.957142857143</v>
       </c>
       <c r="JF11" t="n">
         <v>5662.814285714287</v>
@@ -6811,6 +7552,7 @@
         </is>
       </c>
     </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
@@ -7682,6 +8424,7 @@
         <v>1435</v>
       </c>
     </row>
+    <row r="4"/>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>

</xml_diff>